<commit_message>
used double underscore as field seperator for flattened fields
</commit_message>
<xml_diff>
--- a/excel_reporting_templates/BatteryPass-4.0.0-schema-reporting_template.xlsx
+++ b/excel_reporting_templates/BatteryPass-4.0.0-schema-reporting_template.xlsx
@@ -487,29 +487,29 @@
     <col width="2.4" customWidth="1" min="1" max="1"/>
     <col width="21.6" customWidth="1" min="2" max="2"/>
     <col width="16.8" customWidth="1" min="3" max="3"/>
-    <col width="27.6" customWidth="1" min="4" max="4"/>
-    <col width="24" customWidth="1" min="5" max="5"/>
-    <col width="25.2" customWidth="1" min="6" max="6"/>
-    <col width="28.8" customWidth="1" min="7" max="7"/>
-    <col width="43.2" customWidth="1" min="8" max="8"/>
-    <col width="45.6" customWidth="1" min="9" max="9"/>
-    <col width="44.4" customWidth="1" min="10" max="10"/>
-    <col width="46.8" customWidth="1" min="11" max="11"/>
-    <col width="38.4" customWidth="1" min="12" max="12"/>
-    <col width="40.8" customWidth="1" min="13" max="13"/>
-    <col width="48" customWidth="1" min="14" max="14"/>
-    <col width="39.6" customWidth="1" min="15" max="15"/>
-    <col width="46.8" customWidth="1" min="16" max="16"/>
-    <col width="48" customWidth="1" min="17" max="17"/>
-    <col width="46.8" customWidth="1" min="18" max="18"/>
-    <col width="44.4" customWidth="1" min="19" max="19"/>
+    <col width="28.8" customWidth="1" min="4" max="4"/>
+    <col width="25.2" customWidth="1" min="5" max="5"/>
+    <col width="26.4" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
+    <col width="45.6" customWidth="1" min="8" max="8"/>
+    <col width="48" customWidth="1" min="9" max="9"/>
+    <col width="46.8" customWidth="1" min="10" max="10"/>
+    <col width="49.2" customWidth="1" min="11" max="11"/>
+    <col width="40.8" customWidth="1" min="12" max="12"/>
+    <col width="44.4" customWidth="1" min="13" max="13"/>
+    <col width="50" customWidth="1" min="14" max="14"/>
+    <col width="42" customWidth="1" min="15" max="15"/>
+    <col width="49.2" customWidth="1" min="16" max="16"/>
+    <col width="50" customWidth="1" min="17" max="17"/>
+    <col width="49.2" customWidth="1" min="18" max="18"/>
+    <col width="46.8" customWidth="1" min="19" max="19"/>
     <col width="50" customWidth="1" min="20" max="20"/>
-    <col width="37.2" customWidth="1" min="21" max="21"/>
-    <col width="48" customWidth="1" min="22" max="22"/>
+    <col width="38.4" customWidth="1" min="21" max="21"/>
+    <col width="50" customWidth="1" min="22" max="22"/>
     <col width="50" customWidth="1" min="23" max="23"/>
     <col width="50" customWidth="1" min="24" max="24"/>
-    <col width="49.2" customWidth="1" min="25" max="25"/>
-    <col width="37.2" customWidth="1" min="26" max="26"/>
+    <col width="50" customWidth="1" min="25" max="25"/>
+    <col width="38.4" customWidth="1" min="26" max="26"/>
     <col width="50" customWidth="1" min="27" max="27"/>
     <col width="50" customWidth="1" min="28" max="28"/>
     <col width="50" customWidth="1" min="29" max="29"/>
@@ -536,84 +536,84 @@
     <col width="50" customWidth="1" min="50" max="50"/>
     <col width="50" customWidth="1" min="51" max="51"/>
     <col width="50" customWidth="1" min="52" max="52"/>
-    <col width="43.2" customWidth="1" min="53" max="53"/>
-    <col width="46.8" customWidth="1" min="54" max="54"/>
-    <col width="48" customWidth="1" min="55" max="55"/>
-    <col width="42" customWidth="1" min="56" max="56"/>
-    <col width="42" customWidth="1" min="57" max="57"/>
+    <col width="45.6" customWidth="1" min="53" max="53"/>
+    <col width="49.2" customWidth="1" min="54" max="54"/>
+    <col width="50" customWidth="1" min="55" max="55"/>
+    <col width="44.4" customWidth="1" min="56" max="56"/>
+    <col width="44.4" customWidth="1" min="57" max="57"/>
     <col width="50" customWidth="1" min="58" max="58"/>
     <col width="50" customWidth="1" min="59" max="59"/>
     <col width="50" customWidth="1" min="60" max="60"/>
-    <col width="26.4" customWidth="1" min="61" max="61"/>
-    <col width="21.6" customWidth="1" min="62" max="62"/>
-    <col width="40.8" customWidth="1" min="63" max="63"/>
-    <col width="48" customWidth="1" min="64" max="64"/>
+    <col width="27.6" customWidth="1" min="61" max="61"/>
+    <col width="22.8" customWidth="1" min="62" max="62"/>
+    <col width="42" customWidth="1" min="63" max="63"/>
+    <col width="50" customWidth="1" min="64" max="64"/>
     <col width="50" customWidth="1" min="65" max="65"/>
     <col width="50" customWidth="1" min="66" max="66"/>
-    <col width="42" customWidth="1" min="67" max="67"/>
-    <col width="43.2" customWidth="1" min="68" max="68"/>
-    <col width="40.8" customWidth="1" min="69" max="69"/>
-    <col width="21.6" customWidth="1" min="70" max="70"/>
-    <col width="22.8" customWidth="1" min="71" max="71"/>
-    <col width="18" customWidth="1" min="72" max="72"/>
-    <col width="20.4" customWidth="1" min="73" max="73"/>
-    <col width="34.8" customWidth="1" min="74" max="74"/>
-    <col width="34.8" customWidth="1" min="75" max="75"/>
-    <col width="39.6" customWidth="1" min="76" max="76"/>
-    <col width="44.4" customWidth="1" min="77" max="77"/>
+    <col width="44.4" customWidth="1" min="67" max="67"/>
+    <col width="45.6" customWidth="1" min="68" max="68"/>
+    <col width="43.2" customWidth="1" min="69" max="69"/>
+    <col width="22.8" customWidth="1" min="70" max="70"/>
+    <col width="24" customWidth="1" min="71" max="71"/>
+    <col width="19.2" customWidth="1" min="72" max="72"/>
+    <col width="21.6" customWidth="1" min="73" max="73"/>
+    <col width="38.4" customWidth="1" min="74" max="74"/>
+    <col width="38.4" customWidth="1" min="75" max="75"/>
+    <col width="43.2" customWidth="1" min="76" max="76"/>
+    <col width="48" customWidth="1" min="77" max="77"/>
     <col width="50" customWidth="1" min="78" max="78"/>
     <col width="50" customWidth="1" min="79" max="79"/>
     <col width="50" customWidth="1" min="80" max="80"/>
     <col width="50" customWidth="1" min="81" max="81"/>
-    <col width="36" customWidth="1" min="82" max="82"/>
-    <col width="43.2" customWidth="1" min="83" max="83"/>
-    <col width="39.6" customWidth="1" min="84" max="84"/>
-    <col width="42" customWidth="1" min="85" max="85"/>
-    <col width="39.6" customWidth="1" min="86" max="86"/>
-    <col width="48" customWidth="1" min="87" max="87"/>
-    <col width="34.8" customWidth="1" min="88" max="88"/>
-    <col width="37.2" customWidth="1" min="89" max="89"/>
-    <col width="37.2" customWidth="1" min="90" max="90"/>
-    <col width="42" customWidth="1" min="91" max="91"/>
-    <col width="38.4" customWidth="1" min="92" max="92"/>
+    <col width="39.6" customWidth="1" min="82" max="82"/>
+    <col width="46.8" customWidth="1" min="83" max="83"/>
+    <col width="43.2" customWidth="1" min="84" max="84"/>
+    <col width="45.6" customWidth="1" min="85" max="85"/>
+    <col width="43.2" customWidth="1" min="86" max="86"/>
+    <col width="50" customWidth="1" min="87" max="87"/>
+    <col width="38.4" customWidth="1" min="88" max="88"/>
+    <col width="40.8" customWidth="1" min="89" max="89"/>
+    <col width="40.8" customWidth="1" min="90" max="90"/>
+    <col width="45.6" customWidth="1" min="91" max="91"/>
+    <col width="42" customWidth="1" min="92" max="92"/>
     <col width="50" customWidth="1" min="93" max="93"/>
-    <col width="45.6" customWidth="1" min="94" max="94"/>
+    <col width="49.2" customWidth="1" min="94" max="94"/>
     <col width="50" customWidth="1" min="95" max="95"/>
     <col width="50" customWidth="1" min="96" max="96"/>
     <col width="50" customWidth="1" min="97" max="97"/>
     <col width="50" customWidth="1" min="98" max="98"/>
-    <col width="42" customWidth="1" min="99" max="99"/>
-    <col width="42" customWidth="1" min="100" max="100"/>
-    <col width="44.4" customWidth="1" min="101" max="101"/>
-    <col width="46.8" customWidth="1" min="102" max="102"/>
-    <col width="48" customWidth="1" min="103" max="103"/>
-    <col width="43.2" customWidth="1" min="104" max="104"/>
-    <col width="45.6" customWidth="1" min="105" max="105"/>
-    <col width="48" customWidth="1" min="106" max="106"/>
+    <col width="45.6" customWidth="1" min="99" max="99"/>
+    <col width="45.6" customWidth="1" min="100" max="100"/>
+    <col width="46.8" customWidth="1" min="101" max="101"/>
+    <col width="50" customWidth="1" min="102" max="102"/>
+    <col width="50" customWidth="1" min="103" max="103"/>
+    <col width="46.8" customWidth="1" min="104" max="104"/>
+    <col width="49.2" customWidth="1" min="105" max="105"/>
+    <col width="50" customWidth="1" min="106" max="106"/>
     <col width="50" customWidth="1" min="107" max="107"/>
     <col width="50" customWidth="1" min="108" max="108"/>
-    <col width="49.2" customWidth="1" min="109" max="109"/>
+    <col width="50" customWidth="1" min="109" max="109"/>
     <col width="50" customWidth="1" min="110" max="110"/>
     <col width="50" customWidth="1" min="111" max="111"/>
     <col width="50" customWidth="1" min="112" max="112"/>
     <col width="50" customWidth="1" min="113" max="113"/>
     <col width="50" customWidth="1" min="114" max="114"/>
     <col width="50" customWidth="1" min="115" max="115"/>
-    <col width="46.8" customWidth="1" min="116" max="116"/>
-    <col width="45.6" customWidth="1" min="117" max="117"/>
-    <col width="42" customWidth="1" min="118" max="118"/>
-    <col width="43.2" customWidth="1" min="119" max="119"/>
+    <col width="50" customWidth="1" min="116" max="116"/>
+    <col width="49.2" customWidth="1" min="117" max="117"/>
+    <col width="45.6" customWidth="1" min="118" max="118"/>
+    <col width="46.8" customWidth="1" min="119" max="119"/>
     <col width="50" customWidth="1" min="120" max="120"/>
     <col width="50" customWidth="1" min="121" max="121"/>
     <col width="50" customWidth="1" min="122" max="122"/>
     <col width="50" customWidth="1" min="123" max="123"/>
-    <col width="46.8" customWidth="1" min="124" max="124"/>
-    <col width="43.2" customWidth="1" min="125" max="125"/>
-    <col width="42" customWidth="1" min="126" max="126"/>
-    <col width="48" customWidth="1" min="127" max="127"/>
-    <col width="49.2" customWidth="1" min="128" max="128"/>
-    <col width="46.8" customWidth="1" min="129" max="129"/>
-    <col width="45.6" customWidth="1" min="130" max="130"/>
+    <col width="49.2" customWidth="1" min="124" max="124"/>
+    <col width="48" customWidth="1" min="125" max="125"/>
+    <col width="46.8" customWidth="1" min="126" max="126"/>
+    <col width="50" customWidth="1" min="127" max="127"/>
+    <col width="50" customWidth="1" min="128" max="128"/>
+    <col width="50" customWidth="1" min="129" max="129"/>
+    <col width="50" customWidth="1" min="130" max="130"/>
     <col width="50" customWidth="1" min="131" max="131"/>
     <col width="50" customWidth="1" min="132" max="132"/>
     <col width="50" customWidth="1" min="133" max="133"/>
@@ -634,9 +634,9 @@
     <col width="50" customWidth="1" min="148" max="148"/>
     <col width="50" customWidth="1" min="149" max="149"/>
     <col width="50" customWidth="1" min="150" max="150"/>
-    <col width="44.4" customWidth="1" min="151" max="151"/>
-    <col width="43.2" customWidth="1" min="152" max="152"/>
-    <col width="49.2" customWidth="1" min="153" max="153"/>
+    <col width="49.2" customWidth="1" min="151" max="151"/>
+    <col width="48" customWidth="1" min="152" max="152"/>
+    <col width="50" customWidth="1" min="153" max="153"/>
     <col width="50" customWidth="1" min="154" max="154"/>
     <col width="50" customWidth="1" min="155" max="155"/>
     <col width="50" customWidth="1" min="156" max="156"/>
@@ -648,68 +648,68 @@
     <col width="50" customWidth="1" min="162" max="162"/>
     <col width="50" customWidth="1" min="163" max="163"/>
     <col width="50" customWidth="1" min="164" max="164"/>
-    <col width="43.2" customWidth="1" min="165" max="165"/>
+    <col width="44.4" customWidth="1" min="165" max="165"/>
     <col width="50" customWidth="1" min="166" max="166"/>
     <col width="50" customWidth="1" min="167" max="167"/>
     <col width="50" customWidth="1" min="168" max="168"/>
     <col width="50" customWidth="1" min="169" max="169"/>
-    <col width="48" customWidth="1" min="170" max="170"/>
-    <col width="49.2" customWidth="1" min="171" max="171"/>
-    <col width="44.4" customWidth="1" min="172" max="172"/>
-    <col width="46.8" customWidth="1" min="173" max="173"/>
-    <col width="49.2" customWidth="1" min="174" max="174"/>
+    <col width="50" customWidth="1" min="170" max="170"/>
+    <col width="50" customWidth="1" min="171" max="171"/>
+    <col width="46.8" customWidth="1" min="172" max="172"/>
+    <col width="49.2" customWidth="1" min="173" max="173"/>
+    <col width="50" customWidth="1" min="174" max="174"/>
     <col width="50" customWidth="1" min="175" max="175"/>
-    <col width="45.6" customWidth="1" min="176" max="176"/>
-    <col width="48" customWidth="1" min="177" max="177"/>
-    <col width="48" customWidth="1" min="178" max="178"/>
-    <col width="49.2" customWidth="1" min="179" max="179"/>
-    <col width="44.4" customWidth="1" min="180" max="180"/>
-    <col width="46.8" customWidth="1" min="181" max="181"/>
+    <col width="48" customWidth="1" min="176" max="176"/>
+    <col width="50" customWidth="1" min="177" max="177"/>
+    <col width="50" customWidth="1" min="178" max="178"/>
+    <col width="50" customWidth="1" min="179" max="179"/>
+    <col width="46.8" customWidth="1" min="180" max="180"/>
+    <col width="49.2" customWidth="1" min="181" max="181"/>
     <col width="50" customWidth="1" min="182" max="182"/>
     <col width="50" customWidth="1" min="183" max="183"/>
     <col width="50" customWidth="1" min="184" max="184"/>
     <col width="50" customWidth="1" min="185" max="185"/>
-    <col width="44.4" customWidth="1" min="186" max="186"/>
-    <col width="49.2" customWidth="1" min="187" max="187"/>
-    <col width="38.4" customWidth="1" min="188" max="188"/>
-    <col width="39.6" customWidth="1" min="189" max="189"/>
-    <col width="34.8" customWidth="1" min="190" max="190"/>
-    <col width="37.2" customWidth="1" min="191" max="191"/>
-    <col width="39.6" customWidth="1" min="192" max="192"/>
-    <col width="40.8" customWidth="1" min="193" max="193"/>
-    <col width="36" customWidth="1" min="194" max="194"/>
-    <col width="38.4" customWidth="1" min="195" max="195"/>
-    <col width="39.6" customWidth="1" min="196" max="196"/>
-    <col width="40.8" customWidth="1" min="197" max="197"/>
-    <col width="36" customWidth="1" min="198" max="198"/>
-    <col width="38.4" customWidth="1" min="199" max="199"/>
-    <col width="34.8" customWidth="1" min="200" max="200"/>
-    <col width="36" customWidth="1" min="201" max="201"/>
-    <col width="31.2" customWidth="1" min="202" max="202"/>
-    <col width="33.6" customWidth="1" min="203" max="203"/>
-    <col width="45.6" customWidth="1" min="204" max="204"/>
-    <col width="46.8" customWidth="1" min="205" max="205"/>
-    <col width="42" customWidth="1" min="206" max="206"/>
-    <col width="44.4" customWidth="1" min="207" max="207"/>
-    <col width="36" customWidth="1" min="208" max="208"/>
-    <col width="34.8" customWidth="1" min="209" max="209"/>
-    <col width="36" customWidth="1" min="210" max="210"/>
-    <col width="34.8" customWidth="1" min="211" max="211"/>
-    <col width="36" customWidth="1" min="212" max="212"/>
-    <col width="34.8" customWidth="1" min="213" max="213"/>
-    <col width="38.4" customWidth="1" min="214" max="214"/>
-    <col width="37.2" customWidth="1" min="215" max="215"/>
-    <col width="36" customWidth="1" min="216" max="216"/>
-    <col width="34.8" customWidth="1" min="217" max="217"/>
-    <col width="34.8" customWidth="1" min="218" max="218"/>
-    <col width="33.6" customWidth="1" min="219" max="219"/>
-    <col width="19.2" customWidth="1" min="220" max="220"/>
-    <col width="18" customWidth="1" min="221" max="221"/>
-    <col width="27.6" customWidth="1" min="222" max="222"/>
-    <col width="21.6" customWidth="1" min="223" max="223"/>
+    <col width="46.8" customWidth="1" min="186" max="186"/>
+    <col width="50" customWidth="1" min="187" max="187"/>
+    <col width="40.8" customWidth="1" min="188" max="188"/>
+    <col width="42" customWidth="1" min="189" max="189"/>
+    <col width="37.2" customWidth="1" min="190" max="190"/>
+    <col width="39.6" customWidth="1" min="191" max="191"/>
+    <col width="42" customWidth="1" min="192" max="192"/>
+    <col width="43.2" customWidth="1" min="193" max="193"/>
+    <col width="38.4" customWidth="1" min="194" max="194"/>
+    <col width="40.8" customWidth="1" min="195" max="195"/>
+    <col width="42" customWidth="1" min="196" max="196"/>
+    <col width="43.2" customWidth="1" min="197" max="197"/>
+    <col width="38.4" customWidth="1" min="198" max="198"/>
+    <col width="40.8" customWidth="1" min="199" max="199"/>
+    <col width="37.2" customWidth="1" min="200" max="200"/>
+    <col width="38.4" customWidth="1" min="201" max="201"/>
+    <col width="33.6" customWidth="1" min="202" max="202"/>
+    <col width="36" customWidth="1" min="203" max="203"/>
+    <col width="48" customWidth="1" min="204" max="204"/>
+    <col width="49.2" customWidth="1" min="205" max="205"/>
+    <col width="44.4" customWidth="1" min="206" max="206"/>
+    <col width="46.8" customWidth="1" min="207" max="207"/>
+    <col width="38.4" customWidth="1" min="208" max="208"/>
+    <col width="37.2" customWidth="1" min="209" max="209"/>
+    <col width="38.4" customWidth="1" min="210" max="210"/>
+    <col width="37.2" customWidth="1" min="211" max="211"/>
+    <col width="38.4" customWidth="1" min="212" max="212"/>
+    <col width="37.2" customWidth="1" min="213" max="213"/>
+    <col width="40.8" customWidth="1" min="214" max="214"/>
+    <col width="39.6" customWidth="1" min="215" max="215"/>
+    <col width="38.4" customWidth="1" min="216" max="216"/>
+    <col width="37.2" customWidth="1" min="217" max="217"/>
+    <col width="37.2" customWidth="1" min="218" max="218"/>
+    <col width="36" customWidth="1" min="219" max="219"/>
+    <col width="20.4" customWidth="1" min="220" max="220"/>
+    <col width="19.2" customWidth="1" min="221" max="221"/>
+    <col width="28.8" customWidth="1" min="222" max="222"/>
+    <col width="22.8" customWidth="1" min="223" max="223"/>
     <col width="50" customWidth="1" min="224" max="224"/>
-    <col width="24" customWidth="1" min="225" max="225"/>
-    <col width="32.4" customWidth="1" min="226" max="226"/>
+    <col width="25.2" customWidth="1" min="225" max="225"/>
+    <col width="33.6" customWidth="1" min="226" max="226"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -730,1117 +730,1117 @@
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>identification_category</t>
+          <t>identification__category</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>identification_idDmc</t>
+          <t>identification__idDmc</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>identification_typeId</t>
+          <t>identification__typeId</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>identification_chemistry</t>
+          <t>identification__chemistry</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>identification_additionalCode[0]_key</t>
+          <t>identification__additionalCode[0]__key</t>
         </is>
       </c>
       <c r="I1" s="2" t="inlineStr">
         <is>
-          <t>identification_additionalCode[0]_value</t>
+          <t>identification__additionalCode[0]__value</t>
         </is>
       </c>
       <c r="J1" s="2" t="inlineStr">
         <is>
-          <t>identification_localIdentifier[0]_key</t>
+          <t>identification__localIdentifier[0]__key</t>
         </is>
       </c>
       <c r="K1" s="2" t="inlineStr">
         <is>
-          <t>identification_localIdentifier[0]_value</t>
+          <t>identification__localIdentifier[0]__value</t>
         </is>
       </c>
       <c r="L1" s="2" t="inlineStr">
         <is>
-          <t>identification_typology_longName</t>
+          <t>identification__typology__longName</t>
         </is>
       </c>
       <c r="M1" s="2" t="inlineStr">
         <is>
-          <t>identification_typology_class_code</t>
+          <t>identification__typology__class__code</t>
         </is>
       </c>
       <c r="N1" s="2" t="inlineStr">
         <is>
-          <t>identification_typology_class_definition</t>
+          <t>identification__typology__class__definition</t>
         </is>
       </c>
       <c r="O1" s="2" t="inlineStr">
         <is>
-          <t>identification_typology_shortName</t>
+          <t>identification__typology__shortName</t>
         </is>
       </c>
       <c r="P1" s="2" t="inlineStr">
         <is>
-          <t>chemicalMaterial_activeMaterials_nickel</t>
+          <t>chemicalMaterial__activeMaterials__nickel</t>
         </is>
       </c>
       <c r="Q1" s="2" t="inlineStr">
         <is>
-          <t>chemicalMaterial_activeMaterials_lithium</t>
+          <t>chemicalMaterial__activeMaterials__lithium</t>
         </is>
       </c>
       <c r="R1" s="2" t="inlineStr">
         <is>
-          <t>chemicalMaterial_activeMaterials_cobalt</t>
+          <t>chemicalMaterial__activeMaterials__cobalt</t>
         </is>
       </c>
       <c r="S1" s="2" t="inlineStr">
         <is>
-          <t>chemicalMaterial_activeMaterials_lead</t>
+          <t>chemicalMaterial__activeMaterials__lead</t>
         </is>
       </c>
       <c r="T1" s="3" t="inlineStr">
         <is>
-          <t>chemicalMaterial_activeMaterials_otherMaterials</t>
+          <t>chemicalMaterial__activeMaterials__otherMaterials</t>
         </is>
       </c>
       <c r="U1" s="3" t="inlineStr">
         <is>
-          <t>chemicalMaterial_materialSymbol</t>
+          <t>chemicalMaterial__materialSymbol</t>
         </is>
       </c>
       <c r="V1" s="2" t="inlineStr">
         <is>
-          <t>chemicalMaterial_hazardousSubstance_lead</t>
+          <t>chemicalMaterial__hazardousSubstance__lead</t>
         </is>
       </c>
       <c r="W1" s="2" t="inlineStr">
         <is>
-          <t>chemicalMaterial_hazardousSubstance_cadmium</t>
+          <t>chemicalMaterial__hazardousSubstance__cadmium</t>
         </is>
       </c>
       <c r="X1" s="2" t="inlineStr">
         <is>
-          <t>chemicalMaterial_hazardousSubstance_mercury</t>
+          <t>chemicalMaterial__hazardousSubstance__mercury</t>
         </is>
       </c>
       <c r="Y1" s="3" t="inlineStr">
         <is>
-          <t>chemicalMaterial_hazardousSubstance_other</t>
+          <t>chemicalMaterial__hazardousSubstance__other</t>
         </is>
       </c>
       <c r="Z1" s="2" t="inlineStr">
         <is>
-          <t>chemicalMaterial_otherMaterials</t>
+          <t>chemicalMaterial__otherMaterials</t>
         </is>
       </c>
       <c r="AA1" s="2" t="inlineStr">
         <is>
-          <t>chemicalMaterial_criticalMaterial[0]_criticalName</t>
+          <t>chemicalMaterial__criticalMaterial[0]__criticalName</t>
         </is>
       </c>
       <c r="AB1" s="2" t="inlineStr">
         <is>
-          <t>chemicalMaterial_criticalMaterial[0]_substanceIdentification[0]_materialid</t>
+          <t>chemicalMaterial__criticalMaterial[0]__substanceIdentification[0]__materialid</t>
         </is>
       </c>
       <c r="AC1" s="2" t="inlineStr">
         <is>
-          <t>chemicalMaterial_criticalMaterial[0]_substanceIdentification[0]_type</t>
+          <t>chemicalMaterial__criticalMaterial[0]__substanceIdentification[0]__type</t>
         </is>
       </c>
       <c r="AD1" s="2" t="inlineStr">
         <is>
-          <t>chemicalMaterial_criticalMaterial[0]_substanceName_chemicalName</t>
+          <t>chemicalMaterial__criticalMaterial[0]__substanceName__chemicalName</t>
         </is>
       </c>
       <c r="AE1" s="2" t="inlineStr">
         <is>
-          <t>chemicalMaterial_criticalMaterial[0]_substanceName_type</t>
+          <t>chemicalMaterial__criticalMaterial[0]__substanceName__type</t>
         </is>
       </c>
       <c r="AF1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_separateCollection[0]_content</t>
+          <t>circularity__documents__separateCollection[0]__content</t>
         </is>
       </c>
       <c r="AG1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_separateCollection[0]_category</t>
+          <t>circularity__documents__separateCollection[0]__category</t>
         </is>
       </c>
       <c r="AH1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_separateCollection[0]_type</t>
+          <t>circularity__documents__separateCollection[0]__type</t>
         </is>
       </c>
       <c r="AI1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_separateCollection[0]_header</t>
+          <t>circularity__documents__separateCollection[0]__header</t>
         </is>
       </c>
       <c r="AJ1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_wastePrevention[0]_content</t>
+          <t>circularity__documents__wastePrevention[0]__content</t>
         </is>
       </c>
       <c r="AK1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_wastePrevention[0]_category</t>
+          <t>circularity__documents__wastePrevention[0]__category</t>
         </is>
       </c>
       <c r="AL1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_wastePrevention[0]_type</t>
+          <t>circularity__documents__wastePrevention[0]__type</t>
         </is>
       </c>
       <c r="AM1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_wastePrevention[0]_header</t>
+          <t>circularity__documents__wastePrevention[0]__header</t>
         </is>
       </c>
       <c r="AN1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_impactOfSubstances[0]_content</t>
+          <t>circularity__documents__impactOfSubstances[0]__content</t>
         </is>
       </c>
       <c r="AO1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_impactOfSubstances[0]_category</t>
+          <t>circularity__documents__impactOfSubstances[0]__category</t>
         </is>
       </c>
       <c r="AP1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_impactOfSubstances[0]_type</t>
+          <t>circularity__documents__impactOfSubstances[0]__type</t>
         </is>
       </c>
       <c r="AQ1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_impactOfSubstances[0]_header</t>
+          <t>circularity__documents__impactOfSubstances[0]__header</t>
         </is>
       </c>
       <c r="AR1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_euTaxonomyDisclosureStatement[0]_content</t>
+          <t>circularity__documents__euTaxonomyDisclosureStatement[0]__content</t>
         </is>
       </c>
       <c r="AS1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_euTaxonomyDisclosureStatement[0]_category</t>
+          <t>circularity__documents__euTaxonomyDisclosureStatement[0]__category</t>
         </is>
       </c>
       <c r="AT1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_euTaxonomyDisclosureStatement[0]_type</t>
+          <t>circularity__documents__euTaxonomyDisclosureStatement[0]__type</t>
         </is>
       </c>
       <c r="AU1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_euTaxonomyDisclosureStatement[0]_header</t>
+          <t>circularity__documents__euTaxonomyDisclosureStatement[0]__header</t>
         </is>
       </c>
       <c r="AV1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_sustainabilityReport[0]_content</t>
+          <t>circularity__documents__sustainabilityReport[0]__content</t>
         </is>
       </c>
       <c r="AW1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_sustainabilityReport[0]_category</t>
+          <t>circularity__documents__sustainabilityReport[0]__category</t>
         </is>
       </c>
       <c r="AX1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_sustainabilityReport[0]_type</t>
+          <t>circularity__documents__sustainabilityReport[0]__type</t>
         </is>
       </c>
       <c r="AY1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_sustainabilityReport[0]_header</t>
+          <t>circularity__documents__sustainabilityReport[0]__header</t>
         </is>
       </c>
       <c r="AZ1" s="2" t="inlineStr">
         <is>
-          <t>circularity_documents_separateCollectionSymbol</t>
+          <t>circularity__documents__separateCollectionSymbol</t>
         </is>
       </c>
       <c r="BA1" s="2" t="inlineStr">
         <is>
-          <t>circularity_carbonFootprint[0]_value</t>
+          <t>circularity__carbonFootprint[0]__value</t>
         </is>
       </c>
       <c r="BB1" s="2" t="inlineStr">
         <is>
-          <t>circularity_carbonFootprint[0]_rulebook</t>
+          <t>circularity__carbonFootprint[0]__rulebook</t>
         </is>
       </c>
       <c r="BC1" s="2" t="inlineStr">
         <is>
-          <t>circularity_carbonFootprint[0]_lifecycle</t>
+          <t>circularity__carbonFootprint[0]__lifecycle</t>
         </is>
       </c>
       <c r="BD1" s="2" t="inlineStr">
         <is>
-          <t>circularity_carbonFootprint[0]_unit</t>
+          <t>circularity__carbonFootprint[0]__unit</t>
         </is>
       </c>
       <c r="BE1" s="2" t="inlineStr">
         <is>
-          <t>circularity_carbonFootprint[0]_type</t>
+          <t>circularity__carbonFootprint[0]__type</t>
         </is>
       </c>
       <c r="BF1" s="3" t="inlineStr">
         <is>
-          <t>circularity_carbonFootprint[0]_performanceClass</t>
+          <t>circularity__carbonFootprint[0]__performanceClass</t>
         </is>
       </c>
       <c r="BG1" s="2" t="inlineStr">
         <is>
-          <t>circularity_carbonFootprint[0]_manufacturingPlant</t>
+          <t>circularity__carbonFootprint[0]__manufacturingPlant</t>
         </is>
       </c>
       <c r="BH1" s="2" t="inlineStr">
         <is>
-          <t>circularity_carbonFootprint[0]_declaration</t>
+          <t>circularity__carbonFootprint[0]__declaration</t>
         </is>
       </c>
       <c r="BI1" s="2" t="inlineStr">
         <is>
-          <t>circularity_spareParts</t>
+          <t>circularity__spareParts</t>
         </is>
       </c>
       <c r="BJ1" s="2" t="inlineStr">
         <is>
-          <t>circularity_status</t>
+          <t>circularity__status</t>
         </is>
       </c>
       <c r="BK1" s="3" t="inlineStr">
         <is>
-          <t>generalInformation_intoServiceDate</t>
+          <t>generalInformation__intoServiceDate</t>
         </is>
       </c>
       <c r="BL1" s="2" t="inlineStr">
         <is>
-          <t>generalInformation_manufacturer_facility</t>
+          <t>generalInformation__manufacturer__facility</t>
         </is>
       </c>
       <c r="BM1" s="2" t="inlineStr">
         <is>
-          <t>generalInformation_manufacturer_manufacturer</t>
+          <t>generalInformation__manufacturer__manufacturer</t>
         </is>
       </c>
       <c r="BN1" s="2" t="inlineStr">
         <is>
-          <t>generalInformation_manufacturer_manufacturingDate</t>
+          <t>generalInformation__manufacturer__manufacturingDate</t>
         </is>
       </c>
       <c r="BO1" s="2" t="inlineStr">
         <is>
-          <t>generalInformation_lifespan[0]_unit</t>
+          <t>generalInformation__lifespan[0]__unit</t>
         </is>
       </c>
       <c r="BP1" s="2" t="inlineStr">
         <is>
-          <t>generalInformation_lifespan[0]_value</t>
+          <t>generalInformation__lifespan[0]__value</t>
         </is>
       </c>
       <c r="BQ1" s="2" t="inlineStr">
         <is>
-          <t>generalInformation_lifespan[0]_key</t>
+          <t>generalInformation__lifespan[0]__key</t>
         </is>
       </c>
       <c r="BR1" s="2" t="inlineStr">
         <is>
-          <t>sources[0]_content</t>
+          <t>sources[0]__content</t>
         </is>
       </c>
       <c r="BS1" s="2" t="inlineStr">
         <is>
-          <t>sources[0]_category</t>
+          <t>sources[0]__category</t>
         </is>
       </c>
       <c r="BT1" s="2" t="inlineStr">
         <is>
-          <t>sources[0]_type</t>
+          <t>sources[0]__type</t>
         </is>
       </c>
       <c r="BU1" s="2" t="inlineStr">
         <is>
-          <t>sources[0]_header</t>
+          <t>sources[0]__header</t>
         </is>
       </c>
       <c r="BV1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_voltage_min</t>
+          <t>performance__rated__voltage__min</t>
         </is>
       </c>
       <c r="BW1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_voltage_max</t>
+          <t>performance__rated__voltage__max</t>
         </is>
       </c>
       <c r="BX1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_voltage_nominal</t>
+          <t>performance__rated__voltage__nominal</t>
         </is>
       </c>
       <c r="BY1" s="3" t="inlineStr">
         <is>
-          <t>performance_rated_voltage_temperature</t>
+          <t>performance__rated__voltage__temperature</t>
         </is>
       </c>
       <c r="BZ1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_roundTripEfficiency_depthOfDischarge</t>
+          <t>performance__rated__roundTripEfficiency__depthOfDischarge</t>
         </is>
       </c>
       <c r="CA1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_roundTripEfficiency_initial</t>
+          <t>performance__rated__roundTripEfficiency__initial</t>
         </is>
       </c>
       <c r="CB1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_roundTripEfficiency_50PercentLife</t>
+          <t>performance__rated__roundTripEfficiency__50PercentLife</t>
         </is>
       </c>
       <c r="CC1" s="3" t="inlineStr">
         <is>
-          <t>performance_rated_roundTripEfficiency_temperature</t>
+          <t>performance__rated__roundTripEfficiency__temperature</t>
         </is>
       </c>
       <c r="CD1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_energy_value</t>
+          <t>performance__rated__energy__value</t>
         </is>
       </c>
       <c r="CE1" s="3" t="inlineStr">
         <is>
-          <t>performance_rated_energy_temperature</t>
+          <t>performance__rated__energy__temperature</t>
         </is>
       </c>
       <c r="CF1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_resistance_cell</t>
+          <t>performance__rated__resistance__cell</t>
         </is>
       </c>
       <c r="CG1" s="3" t="inlineStr">
         <is>
-          <t>performance_rated_resistance_module</t>
+          <t>performance__rated__resistance__module</t>
         </is>
       </c>
       <c r="CH1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_resistance_pack</t>
+          <t>performance__rated__resistance__pack</t>
         </is>
       </c>
       <c r="CI1" s="3" t="inlineStr">
         <is>
-          <t>performance_rated_resistance_temperature</t>
+          <t>performance__rated__resistance__temperature</t>
         </is>
       </c>
       <c r="CJ1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_power_value</t>
+          <t>performance__rated__power__value</t>
         </is>
       </c>
       <c r="CK1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_power_at20SoC</t>
+          <t>performance__rated__power__at20SoC</t>
         </is>
       </c>
       <c r="CL1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_power_at80SoC</t>
+          <t>performance__rated__power__at80SoC</t>
         </is>
       </c>
       <c r="CM1" s="3" t="inlineStr">
         <is>
-          <t>performance_rated_power_temperature</t>
+          <t>performance__rated__power__temperature</t>
         </is>
       </c>
       <c r="CN1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_capacity_value</t>
+          <t>performance__rated__capacity__value</t>
         </is>
       </c>
       <c r="CO1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_capacity_thresholdExhaustion</t>
+          <t>performance__rated__capacity__thresholdExhaustion</t>
         </is>
       </c>
       <c r="CP1" s="3" t="inlineStr">
         <is>
-          <t>performance_rated_capacity_temperature</t>
+          <t>performance__rated__capacity__temperature</t>
         </is>
       </c>
       <c r="CQ1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_performanceDocument[0]_content</t>
+          <t>performance__rated__performanceDocument[0]__content</t>
         </is>
       </c>
       <c r="CR1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_performanceDocument[0]_category</t>
+          <t>performance__rated__performanceDocument[0]__category</t>
         </is>
       </c>
       <c r="CS1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_performanceDocument[0]_type</t>
+          <t>performance__rated__performanceDocument[0]__type</t>
         </is>
       </c>
       <c r="CT1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_performanceDocument[0]_header</t>
+          <t>performance__rated__performanceDocument[0]__header</t>
         </is>
       </c>
       <c r="CU1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_temperature_lower</t>
+          <t>performance__rated__temperature__lower</t>
         </is>
       </c>
       <c r="CV1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_temperature_upper</t>
+          <t>performance__rated__temperature__upper</t>
         </is>
       </c>
       <c r="CW1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_selfDischargingRate</t>
+          <t>performance__rated__selfDischargingRate</t>
         </is>
       </c>
       <c r="CX1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_testReport[0]_content</t>
+          <t>performance__rated__testReport[0]__content</t>
         </is>
       </c>
       <c r="CY1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_testReport[0]_category</t>
+          <t>performance__rated__testReport[0]__category</t>
         </is>
       </c>
       <c r="CZ1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_testReport[0]_type</t>
+          <t>performance__rated__testReport[0]__type</t>
         </is>
       </c>
       <c r="DA1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_testReport[0]_header</t>
+          <t>performance__rated__testReport[0]__header</t>
         </is>
       </c>
       <c r="DB1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_expectedYears</t>
+          <t>performance__rated__lifetime__expectedYears</t>
         </is>
       </c>
       <c r="DC1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_report[0]_content</t>
+          <t>performance__rated__lifetime__report[0]__content</t>
         </is>
       </c>
       <c r="DD1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_report[0]_category</t>
+          <t>performance__rated__lifetime__report[0]__category</t>
         </is>
       </c>
       <c r="DE1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_report[0]_type</t>
+          <t>performance__rated__lifetime__report[0]__type</t>
         </is>
       </c>
       <c r="DF1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_report[0]_header</t>
+          <t>performance__rated__lifetime__report[0]__header</t>
         </is>
       </c>
       <c r="DG1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_cycleLifeTesting_temperature</t>
+          <t>performance__rated__lifetime__cycleLifeTesting__temperature</t>
         </is>
       </c>
       <c r="DH1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_cycleLifeTesting_cycles</t>
+          <t>performance__rated__lifetime__cycleLifeTesting__cycles</t>
         </is>
       </c>
       <c r="DI1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_cycleLifeTesting_depthOfDischarge</t>
+          <t>performance__rated__lifetime__cycleLifeTesting__depthOfDischarge</t>
         </is>
       </c>
       <c r="DJ1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_cycleLifeTesting_appliedChargeRate</t>
+          <t>performance__rated__lifetime__cycleLifeTesting__appliedChargeRate</t>
         </is>
       </c>
       <c r="DK1" s="2" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_cycleLifeTesting_appliedDischargeRate</t>
+          <t>performance__rated__lifetime__cycleLifeTesting__appliedDischargeRate</t>
         </is>
       </c>
       <c r="DL1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_stateOfCharge_value</t>
+          <t>performance__dynamic__stateOfCharge__value</t>
         </is>
       </c>
       <c r="DM1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_stateOfCharge_time</t>
+          <t>performance__dynamic__stateOfCharge__time</t>
         </is>
       </c>
       <c r="DN1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_fullCycles_time</t>
+          <t>performance__dynamic__fullCycles__time</t>
         </is>
       </c>
       <c r="DO1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_fullCycles_value</t>
+          <t>performance__dynamic__fullCycles__value</t>
         </is>
       </c>
       <c r="DP1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_performanceDocument[0]_content</t>
+          <t>performance__dynamic__performanceDocument[0]__content</t>
         </is>
       </c>
       <c r="DQ1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_performanceDocument[0]_category</t>
+          <t>performance__dynamic__performanceDocument[0]__category</t>
         </is>
       </c>
       <c r="DR1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_performanceDocument[0]_type</t>
+          <t>performance__dynamic__performanceDocument[0]__type</t>
         </is>
       </c>
       <c r="DS1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_performanceDocument[0]_header</t>
+          <t>performance__dynamic__performanceDocument[0]__header</t>
         </is>
       </c>
       <c r="DT1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_selfDischargingRate</t>
+          <t>performance__dynamic__selfDischargingRate</t>
         </is>
       </c>
       <c r="DU1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_power_fade_value</t>
+          <t>performance__dynamic__power__fade__value</t>
         </is>
       </c>
       <c r="DV1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_power_fade_time</t>
+          <t>performance__dynamic__power__fade__time</t>
         </is>
       </c>
       <c r="DW1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_power_remaining_time</t>
+          <t>performance__dynamic__power__remaining__time</t>
         </is>
       </c>
       <c r="DX1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_power_remaining_value</t>
+          <t>performance__dynamic__power__remaining__value</t>
         </is>
       </c>
       <c r="DY1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_capacity_fade_value</t>
+          <t>performance__dynamic__capacity__fade__value</t>
         </is>
       </c>
       <c r="DZ1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_capacity_fade_time</t>
+          <t>performance__dynamic__capacity__fade__time</t>
         </is>
       </c>
       <c r="EA1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_capacity_throughput_time</t>
+          <t>performance__dynamic__capacity__throughput__time</t>
         </is>
       </c>
       <c r="EB1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_capacity_throughput_value</t>
+          <t>performance__dynamic__capacity__throughput__value</t>
         </is>
       </c>
       <c r="EC1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_capacity_capacity_time</t>
+          <t>performance__dynamic__capacity__capacity__time</t>
         </is>
       </c>
       <c r="ED1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_capacity_capacity_value</t>
+          <t>performance__dynamic__capacity__capacity__value</t>
         </is>
       </c>
       <c r="EE1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_roundTripEfficiency_fade_value</t>
+          <t>performance__dynamic__roundTripEfficiency__fade__value</t>
         </is>
       </c>
       <c r="EF1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_roundTripEfficiency_fade_time</t>
+          <t>performance__dynamic__roundTripEfficiency__fade__time</t>
         </is>
       </c>
       <c r="EG1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_roundTripEfficiency_remaining_value</t>
+          <t>performance__dynamic__roundTripEfficiency__remaining__value</t>
         </is>
       </c>
       <c r="EH1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_roundTripEfficiency_remaining_time</t>
+          <t>performance__dynamic__roundTripEfficiency__remaining__time</t>
         </is>
       </c>
       <c r="EI1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_increase_pack_value</t>
+          <t>performance__dynamic__resistance__increase__pack__value</t>
         </is>
       </c>
       <c r="EJ1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_increase_pack_time</t>
+          <t>performance__dynamic__resistance__increase__pack__time</t>
         </is>
       </c>
       <c r="EK1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_increase_module_value</t>
+          <t>performance__dynamic__resistance__increase__module__value</t>
         </is>
       </c>
       <c r="EL1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_increase_module_time</t>
+          <t>performance__dynamic__resistance__increase__module__time</t>
         </is>
       </c>
       <c r="EM1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_increase_cell_value</t>
+          <t>performance__dynamic__resistance__increase__cell__value</t>
         </is>
       </c>
       <c r="EN1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_increase_cell_time</t>
+          <t>performance__dynamic__resistance__increase__cell__time</t>
         </is>
       </c>
       <c r="EO1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_remaining_pack_time</t>
+          <t>performance__dynamic__resistance__remaining__pack__time</t>
         </is>
       </c>
       <c r="EP1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_remaining_pack_value</t>
+          <t>performance__dynamic__resistance__remaining__pack__value</t>
         </is>
       </c>
       <c r="EQ1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_remaining_module_time</t>
+          <t>performance__dynamic__resistance__remaining__module__time</t>
         </is>
       </c>
       <c r="ER1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_remaining_module_value</t>
+          <t>performance__dynamic__resistance__remaining__module__value</t>
         </is>
       </c>
       <c r="ES1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_remaining_cell_time</t>
+          <t>performance__dynamic__resistance__remaining__cell__time</t>
         </is>
       </c>
       <c r="ET1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_remaining_cell_value</t>
+          <t>performance__dynamic__resistance__remaining__cell__value</t>
         </is>
       </c>
       <c r="EU1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_energy_soce_value</t>
+          <t>performance__dynamic__energy__soce__value</t>
         </is>
       </c>
       <c r="EV1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_energy_soce_time</t>
+          <t>performance__dynamic__energy__soce__time</t>
         </is>
       </c>
       <c r="EW1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_energy_remaining_time</t>
+          <t>performance__dynamic__energy__remaining__time</t>
         </is>
       </c>
       <c r="EX1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_energy_remaining_value</t>
+          <t>performance__dynamic__energy__remaining__value</t>
         </is>
       </c>
       <c r="EY1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_energy_throughput_time</t>
+          <t>performance__dynamic__energy__throughput__time</t>
         </is>
       </c>
       <c r="EZ1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_energy_throughput_value</t>
+          <t>performance__dynamic__energy__throughput__value</t>
         </is>
       </c>
       <c r="FA1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_negativeEvents[0]_content</t>
+          <t>performance__dynamic__negativeEvents[0]__content</t>
         </is>
       </c>
       <c r="FB1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_negativeEvents[0]_category</t>
+          <t>performance__dynamic__negativeEvents[0]__category</t>
         </is>
       </c>
       <c r="FC1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_negativeEvents[0]_type</t>
+          <t>performance__dynamic__negativeEvents[0]__type</t>
         </is>
       </c>
       <c r="FD1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_negativeEvents[0]_header</t>
+          <t>performance__dynamic__negativeEvents[0]__header</t>
         </is>
       </c>
       <c r="FE1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_operatingEnvironment[0]_content</t>
+          <t>performance__dynamic__operatingEnvironment[0]__content</t>
         </is>
       </c>
       <c r="FF1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_operatingEnvironment[0]_category</t>
+          <t>performance__dynamic__operatingEnvironment[0]__category</t>
         </is>
       </c>
       <c r="FG1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_operatingEnvironment[0]_type</t>
+          <t>performance__dynamic__operatingEnvironment[0]__type</t>
         </is>
       </c>
       <c r="FH1" s="2" t="inlineStr">
         <is>
-          <t>performance_dynamic_operatingEnvironment[0]_header</t>
+          <t>performance__dynamic__operatingEnvironment[0]__header</t>
         </is>
       </c>
       <c r="FI1" s="3" t="inlineStr">
         <is>
-          <t>conformity_declarationOfConformityId</t>
+          <t>conformity__declarationOfConformityId</t>
         </is>
       </c>
       <c r="FJ1" s="2" t="inlineStr">
         <is>
-          <t>conformity_declarationOfConformity[0]_content</t>
+          <t>conformity__declarationOfConformity[0]__content</t>
         </is>
       </c>
       <c r="FK1" s="2" t="inlineStr">
         <is>
-          <t>conformity_declarationOfConformity[0]_category</t>
+          <t>conformity__declarationOfConformity[0]__category</t>
         </is>
       </c>
       <c r="FL1" s="2" t="inlineStr">
         <is>
-          <t>conformity_declarationOfConformity[0]_type</t>
+          <t>conformity__declarationOfConformity[0]__type</t>
         </is>
       </c>
       <c r="FM1" s="2" t="inlineStr">
         <is>
-          <t>conformity_declarationOfConformity[0]_header</t>
+          <t>conformity__declarationOfConformity[0]__header</t>
         </is>
       </c>
       <c r="FN1" s="2" t="inlineStr">
         <is>
-          <t>conformity_resultOfTestReport[0]_content</t>
+          <t>conformity__resultOfTestReport[0]__content</t>
         </is>
       </c>
       <c r="FO1" s="2" t="inlineStr">
         <is>
-          <t>conformity_resultOfTestReport[0]_category</t>
+          <t>conformity__resultOfTestReport[0]__category</t>
         </is>
       </c>
       <c r="FP1" s="2" t="inlineStr">
         <is>
-          <t>conformity_resultOfTestReport[0]_type</t>
+          <t>conformity__resultOfTestReport[0]__type</t>
         </is>
       </c>
       <c r="FQ1" s="2" t="inlineStr">
         <is>
-          <t>conformity_resultOfTestReport[0]_header</t>
+          <t>conformity__resultOfTestReport[0]__header</t>
         </is>
       </c>
       <c r="FR1" s="2" t="inlineStr">
         <is>
-          <t>conformity_thirdPartyAssurance[0]_content</t>
+          <t>conformity__thirdPartyAssurance[0]__content</t>
         </is>
       </c>
       <c r="FS1" s="2" t="inlineStr">
         <is>
-          <t>conformity_thirdPartyAssurance[0]_category</t>
+          <t>conformity__thirdPartyAssurance[0]__category</t>
         </is>
       </c>
       <c r="FT1" s="2" t="inlineStr">
         <is>
-          <t>conformity_thirdPartyAssurance[0]_type</t>
+          <t>conformity__thirdPartyAssurance[0]__type</t>
         </is>
       </c>
       <c r="FU1" s="2" t="inlineStr">
         <is>
-          <t>conformity_thirdPartyAssurance[0]_header</t>
+          <t>conformity__thirdPartyAssurance[0]__header</t>
         </is>
       </c>
       <c r="FV1" s="2" t="inlineStr">
         <is>
-          <t>conformity_dueDiligencePolicy[0]_content</t>
+          <t>conformity__dueDiligencePolicy[0]__content</t>
         </is>
       </c>
       <c r="FW1" s="2" t="inlineStr">
         <is>
-          <t>conformity_dueDiligencePolicy[0]_category</t>
+          <t>conformity__dueDiligencePolicy[0]__category</t>
         </is>
       </c>
       <c r="FX1" s="2" t="inlineStr">
         <is>
-          <t>conformity_dueDiligencePolicy[0]_type</t>
+          <t>conformity__dueDiligencePolicy[0]__type</t>
         </is>
       </c>
       <c r="FY1" s="2" t="inlineStr">
         <is>
-          <t>conformity_dueDiligencePolicy[0]_header</t>
+          <t>conformity__dueDiligencePolicy[0]__header</t>
         </is>
       </c>
       <c r="FZ1" s="2" t="inlineStr">
         <is>
-          <t>safety_usableExtinguishAgent[0]_document[0]_content</t>
+          <t>safety__usableExtinguishAgent[0]__document[0]__content</t>
         </is>
       </c>
       <c r="GA1" s="2" t="inlineStr">
         <is>
-          <t>safety_usableExtinguishAgent[0]_document[0]_category</t>
+          <t>safety__usableExtinguishAgent[0]__document[0]__category</t>
         </is>
       </c>
       <c r="GB1" s="2" t="inlineStr">
         <is>
-          <t>safety_usableExtinguishAgent[0]_document[0]_type</t>
+          <t>safety__usableExtinguishAgent[0]__document[0]__type</t>
         </is>
       </c>
       <c r="GC1" s="2" t="inlineStr">
         <is>
-          <t>safety_usableExtinguishAgent[0]_document[0]_header</t>
+          <t>safety__usableExtinguishAgent[0]__document[0]__header</t>
         </is>
       </c>
       <c r="GD1" s="2" t="inlineStr">
         <is>
-          <t>safety_usableExtinguishAgent[0]_media</t>
+          <t>safety__usableExtinguishAgent[0]__media</t>
         </is>
       </c>
       <c r="GE1" s="2" t="inlineStr">
         <is>
-          <t>safety_usableExtinguishAgent[0]_fireClass</t>
+          <t>safety__usableExtinguishAgent[0]__fireClass</t>
         </is>
       </c>
       <c r="GF1" s="2" t="inlineStr">
         <is>
-          <t>safety_safetyMeasures[0]_content</t>
+          <t>safety__safetyMeasures[0]__content</t>
         </is>
       </c>
       <c r="GG1" s="2" t="inlineStr">
         <is>
-          <t>safety_safetyMeasures[0]_category</t>
+          <t>safety__safetyMeasures[0]__category</t>
         </is>
       </c>
       <c r="GH1" s="2" t="inlineStr">
         <is>
-          <t>safety_safetyMeasures[0]_type</t>
+          <t>safety__safetyMeasures[0]__type</t>
         </is>
       </c>
       <c r="GI1" s="2" t="inlineStr">
         <is>
-          <t>safety_safetyMeasures[0]_header</t>
+          <t>safety__safetyMeasures[0]__header</t>
         </is>
       </c>
       <c r="GJ1" s="2" t="inlineStr">
         <is>
-          <t>safety_meaningOfLabels[0]_content</t>
+          <t>safety__meaningOfLabels[0]__content</t>
         </is>
       </c>
       <c r="GK1" s="2" t="inlineStr">
         <is>
-          <t>safety_meaningOfLabels[0]_category</t>
+          <t>safety__meaningOfLabels[0]__category</t>
         </is>
       </c>
       <c r="GL1" s="2" t="inlineStr">
         <is>
-          <t>safety_meaningOfLabels[0]_type</t>
+          <t>safety__meaningOfLabels[0]__type</t>
         </is>
       </c>
       <c r="GM1" s="2" t="inlineStr">
         <is>
-          <t>safety_meaningOfLabels[0]_header</t>
+          <t>safety__meaningOfLabels[0]__header</t>
         </is>
       </c>
       <c r="GN1" s="2" t="inlineStr">
         <is>
-          <t>safety_safeDischarging[0]_content</t>
+          <t>safety__safeDischarging[0]__content</t>
         </is>
       </c>
       <c r="GO1" s="2" t="inlineStr">
         <is>
-          <t>safety_safeDischarging[0]_category</t>
+          <t>safety__safeDischarging[0]__category</t>
         </is>
       </c>
       <c r="GP1" s="2" t="inlineStr">
         <is>
-          <t>safety_safeDischarging[0]_type</t>
+          <t>safety__safeDischarging[0]__type</t>
         </is>
       </c>
       <c r="GQ1" s="2" t="inlineStr">
         <is>
-          <t>safety_safeDischarging[0]_header</t>
+          <t>safety__safeDischarging[0]__header</t>
         </is>
       </c>
       <c r="GR1" s="2" t="inlineStr">
         <is>
-          <t>safety_dismantling[0]_content</t>
+          <t>safety__dismantling[0]__content</t>
         </is>
       </c>
       <c r="GS1" s="2" t="inlineStr">
         <is>
-          <t>safety_dismantling[0]_category</t>
+          <t>safety__dismantling[0]__category</t>
         </is>
       </c>
       <c r="GT1" s="2" t="inlineStr">
         <is>
-          <t>safety_dismantling[0]_type</t>
+          <t>safety__dismantling[0]__type</t>
         </is>
       </c>
       <c r="GU1" s="2" t="inlineStr">
         <is>
-          <t>safety_dismantling[0]_header</t>
+          <t>safety__dismantling[0]__header</t>
         </is>
       </c>
       <c r="GV1" s="2" t="inlineStr">
         <is>
-          <t>safety_removalFromAppliance[0]_content</t>
+          <t>safety__removalFromAppliance[0]__content</t>
         </is>
       </c>
       <c r="GW1" s="2" t="inlineStr">
         <is>
-          <t>safety_removalFromAppliance[0]_category</t>
+          <t>safety__removalFromAppliance[0]__category</t>
         </is>
       </c>
       <c r="GX1" s="2" t="inlineStr">
         <is>
-          <t>safety_removalFromAppliance[0]_type</t>
+          <t>safety__removalFromAppliance[0]__type</t>
         </is>
       </c>
       <c r="GY1" s="2" t="inlineStr">
         <is>
-          <t>safety_removalFromAppliance[0]_header</t>
+          <t>safety__removalFromAppliance[0]__header</t>
         </is>
       </c>
       <c r="GZ1" s="2" t="inlineStr">
         <is>
-          <t>physicalDimension_weight_value</t>
+          <t>physicalDimension__weight__value</t>
         </is>
       </c>
       <c r="HA1" s="2" t="inlineStr">
         <is>
-          <t>physicalDimension_weight_unit</t>
+          <t>physicalDimension__weight__unit</t>
         </is>
       </c>
       <c r="HB1" s="2" t="inlineStr">
         <is>
-          <t>physicalDimension_volume_value</t>
+          <t>physicalDimension__volume__value</t>
         </is>
       </c>
       <c r="HC1" s="2" t="inlineStr">
         <is>
-          <t>physicalDimension_volume_unit</t>
+          <t>physicalDimension__volume__unit</t>
         </is>
       </c>
       <c r="HD1" s="2" t="inlineStr">
         <is>
-          <t>physicalDimension_height_value</t>
+          <t>physicalDimension__height__value</t>
         </is>
       </c>
       <c r="HE1" s="2" t="inlineStr">
         <is>
-          <t>physicalDimension_height_unit</t>
+          <t>physicalDimension__height__unit</t>
         </is>
       </c>
       <c r="HF1" s="2" t="inlineStr">
         <is>
-          <t>physicalDimension_diameter_value</t>
+          <t>physicalDimension__diameter__value</t>
         </is>
       </c>
       <c r="HG1" s="2" t="inlineStr">
         <is>
-          <t>physicalDimension_diameter_unit</t>
+          <t>physicalDimension__diameter__unit</t>
         </is>
       </c>
       <c r="HH1" s="2" t="inlineStr">
         <is>
-          <t>physicalDimension_length_value</t>
+          <t>physicalDimension__length__value</t>
         </is>
       </c>
       <c r="HI1" s="2" t="inlineStr">
         <is>
-          <t>physicalDimension_length_unit</t>
+          <t>physicalDimension__length__unit</t>
         </is>
       </c>
       <c r="HJ1" s="2" t="inlineStr">
         <is>
-          <t>physicalDimension_width_value</t>
+          <t>physicalDimension__width__value</t>
         </is>
       </c>
       <c r="HK1" s="2" t="inlineStr">
         <is>
-          <t>physicalDimension_width_unit</t>
+          <t>physicalDimension__width__unit</t>
         </is>
       </c>
       <c r="HL1" s="2" t="inlineStr">
         <is>
-          <t>metadata_version</t>
+          <t>metadata__version</t>
         </is>
       </c>
       <c r="HM1" s="3" t="inlineStr">
         <is>
-          <t>metadata_status</t>
+          <t>metadata__status</t>
         </is>
       </c>
       <c r="HN1" s="2" t="inlineStr">
         <is>
-          <t>metadata_expirationDate</t>
+          <t>metadata__expirationDate</t>
         </is>
       </c>
       <c r="HO1" s="2" t="inlineStr">
         <is>
-          <t>metadata_issueDate</t>
+          <t>metadata__issueDate</t>
         </is>
       </c>
       <c r="HP1" s="2" t="inlineStr">
         <is>
-          <t>metadata_economicOperator_economicOperatorId</t>
+          <t>metadata__economicOperator__economicOperatorId</t>
         </is>
       </c>
       <c r="HQ1" s="2" t="inlineStr">
         <is>
-          <t>metadata_predecessor</t>
+          <t>metadata__predecessor</t>
         </is>
       </c>
       <c r="HR1" s="2" t="inlineStr">
         <is>
-          <t>metadata_passportIdentifier</t>
+          <t>metadata__passportIdentifier</t>
         </is>
       </c>
     </row>
@@ -1889,7 +1889,7 @@
     <row r="3" ht="30" customHeight="1">
       <c r="A3" s="4" t="inlineStr">
         <is>
-          <t>2. Columns highlighted in olive green are digital twin fields.</t>
+          <t>1. Columns highlighted in olive green are digital twin fields.</t>
         </is>
       </c>
       <c r="B3" s="5" t="n"/>
@@ -1920,7 +1920,7 @@
       </c>
       <c r="B5" s="7" t="inlineStr">
         <is>
-          <t>Digital Twin Field: id</t>
+          <t>Digital Twin Field Name: id</t>
         </is>
       </c>
       <c r="C5" s="7" t="n"/>
@@ -1933,7 +1933,7 @@
       </c>
       <c r="B6" s="8" t="inlineStr">
         <is>
-          <t>Digital Twin Field: manufacturerPartId</t>
+          <t>Digital Twin Field Name: manufacturerPartId</t>
         </is>
       </c>
       <c r="C6" s="8" t="n"/>
@@ -1946,7 +1946,7 @@
       </c>
       <c r="B7" s="7" t="inlineStr">
         <is>
-          <t>Digital Twin Field: partInstanceId</t>
+          <t>Digital Twin Field Name: partInstanceId</t>
         </is>
       </c>
       <c r="C7" s="7" t="n"/>
@@ -1954,7 +1954,7 @@
     <row r="8">
       <c r="A8" s="8" t="inlineStr">
         <is>
-          <t>identification_category</t>
+          <t>identification__category</t>
         </is>
       </c>
       <c r="B8" s="8" t="inlineStr">
@@ -1972,7 +1972,7 @@
     <row r="9">
       <c r="A9" s="7" t="inlineStr">
         <is>
-          <t>identification_idDmc</t>
+          <t>identification__idDmc</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1989,7 +1989,7 @@
     <row r="10">
       <c r="A10" s="8" t="inlineStr">
         <is>
-          <t>identification_typeId</t>
+          <t>identification__typeId</t>
         </is>
       </c>
       <c r="B10" s="8" t="inlineStr">
@@ -2005,7 +2005,7 @@
     <row r="11">
       <c r="A11" s="7" t="inlineStr">
         <is>
-          <t>identification_chemistry</t>
+          <t>identification__chemistry</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -2019,7 +2019,7 @@
     <row r="12">
       <c r="A12" s="8" t="inlineStr">
         <is>
-          <t>identification_additionalCode[0]_key</t>
+          <t>identification__additionalCode[0]__key</t>
         </is>
       </c>
       <c r="B12" s="8" t="inlineStr">
@@ -2039,7 +2039,7 @@
     <row r="13">
       <c r="A13" s="7" t="inlineStr">
         <is>
-          <t>identification_additionalCode[0]_value</t>
+          <t>identification__additionalCode[0]__value</t>
         </is>
       </c>
       <c r="B13" s="7" t="inlineStr">
@@ -2052,7 +2052,7 @@
     <row r="14">
       <c r="A14" s="8" t="inlineStr">
         <is>
-          <t>identification_localIdentifier[0]_key</t>
+          <t>identification__localIdentifier[0]__key</t>
         </is>
       </c>
       <c r="B14" s="8" t="inlineStr">
@@ -2072,7 +2072,7 @@
     <row r="15">
       <c r="A15" s="7" t="inlineStr">
         <is>
-          <t>identification_localIdentifier[0]_value</t>
+          <t>identification__localIdentifier[0]__value</t>
         </is>
       </c>
       <c r="B15" s="7" t="inlineStr">
@@ -2088,7 +2088,7 @@
     <row r="16">
       <c r="A16" s="8" t="inlineStr">
         <is>
-          <t>identification_typology_longName</t>
+          <t>identification__typology__longName</t>
         </is>
       </c>
       <c r="B16" s="8" t="inlineStr">
@@ -2101,7 +2101,7 @@
     <row r="17">
       <c r="A17" s="7" t="inlineStr">
         <is>
-          <t>identification_typology_class_code</t>
+          <t>identification__typology__class__code</t>
         </is>
       </c>
       <c r="B17" s="7" t="inlineStr">
@@ -2114,7 +2114,7 @@
     <row r="18">
       <c r="A18" s="8" t="inlineStr">
         <is>
-          <t>identification_typology_class_definition</t>
+          <t>identification__typology__class__definition</t>
         </is>
       </c>
       <c r="B18" s="8" t="inlineStr">
@@ -2127,7 +2127,7 @@
     <row r="19">
       <c r="A19" s="7" t="inlineStr">
         <is>
-          <t>identification_typology_shortName</t>
+          <t>identification__typology__shortName</t>
         </is>
       </c>
       <c r="B19" s="7" t="inlineStr">
@@ -2140,7 +2140,7 @@
     <row r="20">
       <c r="A20" s="8" t="inlineStr">
         <is>
-          <t>chemicalMaterial_activeMaterials_nickel</t>
+          <t>chemicalMaterial__activeMaterials__nickel</t>
         </is>
       </c>
       <c r="B20" s="8" t="inlineStr">
@@ -2154,7 +2154,7 @@
     <row r="21">
       <c r="A21" s="7" t="inlineStr">
         <is>
-          <t>chemicalMaterial_activeMaterials_lithium</t>
+          <t>chemicalMaterial__activeMaterials__lithium</t>
         </is>
       </c>
       <c r="B21" s="7" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="22">
       <c r="A22" s="8" t="inlineStr">
         <is>
-          <t>chemicalMaterial_activeMaterials_cobalt</t>
+          <t>chemicalMaterial__activeMaterials__cobalt</t>
         </is>
       </c>
       <c r="B22" s="8" t="inlineStr">
@@ -2182,7 +2182,7 @@
     <row r="23">
       <c r="A23" s="7" t="inlineStr">
         <is>
-          <t>chemicalMaterial_activeMaterials_lead</t>
+          <t>chemicalMaterial__activeMaterials__lead</t>
         </is>
       </c>
       <c r="B23" s="7" t="inlineStr">
@@ -2196,7 +2196,7 @@
     <row r="24">
       <c r="A24" s="8" t="inlineStr">
         <is>
-          <t>chemicalMaterial_activeMaterials_otherMaterials</t>
+          <t>chemicalMaterial__activeMaterials__otherMaterials</t>
         </is>
       </c>
       <c r="B24" s="8" t="inlineStr">
@@ -2219,7 +2219,7 @@
     <row r="25">
       <c r="A25" s="7" t="inlineStr">
         <is>
-          <t>chemicalMaterial_materialSymbol</t>
+          <t>chemicalMaterial__materialSymbol</t>
         </is>
       </c>
       <c r="B25" s="7" t="inlineStr">
@@ -2233,7 +2233,7 @@
     <row r="26">
       <c r="A26" s="8" t="inlineStr">
         <is>
-          <t>chemicalMaterial_hazardousSubstance_lead</t>
+          <t>chemicalMaterial__hazardousSubstance__lead</t>
         </is>
       </c>
       <c r="B26" s="8" t="inlineStr">
@@ -2249,7 +2249,7 @@
     <row r="27">
       <c r="A27" s="7" t="inlineStr">
         <is>
-          <t>chemicalMaterial_hazardousSubstance_cadmium</t>
+          <t>chemicalMaterial__hazardousSubstance__cadmium</t>
         </is>
       </c>
       <c r="B27" s="7" t="inlineStr">
@@ -2265,7 +2265,7 @@
     <row r="28">
       <c r="A28" s="8" t="inlineStr">
         <is>
-          <t>chemicalMaterial_hazardousSubstance_mercury</t>
+          <t>chemicalMaterial__hazardousSubstance__mercury</t>
         </is>
       </c>
       <c r="B28" s="8" t="inlineStr">
@@ -2281,7 +2281,7 @@
     <row r="29">
       <c r="A29" s="7" t="inlineStr">
         <is>
-          <t>chemicalMaterial_hazardousSubstance_other</t>
+          <t>chemicalMaterial__hazardousSubstance__other</t>
         </is>
       </c>
       <c r="B29" s="7" t="inlineStr">
@@ -2304,7 +2304,7 @@
     <row r="30">
       <c r="A30" s="8" t="inlineStr">
         <is>
-          <t>chemicalMaterial_otherMaterials</t>
+          <t>chemicalMaterial__otherMaterials</t>
         </is>
       </c>
       <c r="B30" s="8" t="inlineStr">
@@ -2327,7 +2327,7 @@
     <row r="31">
       <c r="A31" s="7" t="inlineStr">
         <is>
-          <t>chemicalMaterial_criticalMaterial[0]_criticalName</t>
+          <t>chemicalMaterial__criticalMaterial[0]__criticalName</t>
         </is>
       </c>
       <c r="B31" s="7" t="inlineStr">
@@ -2341,7 +2341,7 @@
     <row r="32">
       <c r="A32" s="8" t="inlineStr">
         <is>
-          <t>chemicalMaterial_criticalMaterial[0]_substanceIdentification[0]_materialid</t>
+          <t>chemicalMaterial__criticalMaterial[0]__substanceIdentification[0]__materialid</t>
         </is>
       </c>
       <c r="B32" s="8" t="inlineStr">
@@ -2354,7 +2354,7 @@
     <row r="33">
       <c r="A33" s="7" t="inlineStr">
         <is>
-          <t>chemicalMaterial_criticalMaterial[0]_substanceIdentification[0]_type</t>
+          <t>chemicalMaterial__criticalMaterial[0]__substanceIdentification[0]__type</t>
         </is>
       </c>
       <c r="B33" s="7" t="inlineStr">
@@ -2371,7 +2371,7 @@
     <row r="34">
       <c r="A34" s="8" t="inlineStr">
         <is>
-          <t>chemicalMaterial_criticalMaterial[0]_substanceName_chemicalName</t>
+          <t>chemicalMaterial__criticalMaterial[0]__substanceName__chemicalName</t>
         </is>
       </c>
       <c r="B34" s="8" t="inlineStr">
@@ -2384,7 +2384,7 @@
     <row r="35">
       <c r="A35" s="7" t="inlineStr">
         <is>
-          <t>chemicalMaterial_criticalMaterial[0]_substanceName_type</t>
+          <t>chemicalMaterial__criticalMaterial[0]__substanceName__type</t>
         </is>
       </c>
       <c r="B35" s="7" t="inlineStr">
@@ -2401,7 +2401,7 @@
     <row r="36">
       <c r="A36" s="8" t="inlineStr">
         <is>
-          <t>circularity_documents_separateCollection[0]_content</t>
+          <t>circularity__documents__separateCollection[0]__content</t>
         </is>
       </c>
       <c r="B36" s="8" t="inlineStr">
@@ -2414,7 +2414,7 @@
     <row r="37">
       <c r="A37" s="7" t="inlineStr">
         <is>
-          <t>circularity_documents_separateCollection[0]_category</t>
+          <t>circularity__documents__separateCollection[0]__category</t>
         </is>
       </c>
       <c r="B37" s="7" t="inlineStr">
@@ -2442,7 +2442,7 @@
     <row r="38">
       <c r="A38" s="8" t="inlineStr">
         <is>
-          <t>circularity_documents_separateCollection[0]_type</t>
+          <t>circularity__documents__separateCollection[0]__type</t>
         </is>
       </c>
       <c r="B38" s="8" t="inlineStr">
@@ -2459,7 +2459,7 @@
     <row r="39">
       <c r="A39" s="7" t="inlineStr">
         <is>
-          <t>circularity_documents_separateCollection[0]_header</t>
+          <t>circularity__documents__separateCollection[0]__header</t>
         </is>
       </c>
       <c r="B39" s="7" t="inlineStr">
@@ -2472,7 +2472,7 @@
     <row r="40">
       <c r="A40" s="8" t="inlineStr">
         <is>
-          <t>circularity_documents_wastePrevention[0]_content</t>
+          <t>circularity__documents__wastePrevention[0]__content</t>
         </is>
       </c>
       <c r="B40" s="8" t="inlineStr">
@@ -2485,7 +2485,7 @@
     <row r="41">
       <c r="A41" s="7" t="inlineStr">
         <is>
-          <t>circularity_documents_wastePrevention[0]_category</t>
+          <t>circularity__documents__wastePrevention[0]__category</t>
         </is>
       </c>
       <c r="B41" s="7" t="inlineStr">
@@ -2513,7 +2513,7 @@
     <row r="42">
       <c r="A42" s="8" t="inlineStr">
         <is>
-          <t>circularity_documents_wastePrevention[0]_type</t>
+          <t>circularity__documents__wastePrevention[0]__type</t>
         </is>
       </c>
       <c r="B42" s="8" t="inlineStr">
@@ -2530,7 +2530,7 @@
     <row r="43">
       <c r="A43" s="7" t="inlineStr">
         <is>
-          <t>circularity_documents_wastePrevention[0]_header</t>
+          <t>circularity__documents__wastePrevention[0]__header</t>
         </is>
       </c>
       <c r="B43" s="7" t="inlineStr">
@@ -2543,7 +2543,7 @@
     <row r="44">
       <c r="A44" s="8" t="inlineStr">
         <is>
-          <t>circularity_documents_impactOfSubstances[0]_content</t>
+          <t>circularity__documents__impactOfSubstances[0]__content</t>
         </is>
       </c>
       <c r="B44" s="8" t="inlineStr">
@@ -2556,7 +2556,7 @@
     <row r="45">
       <c r="A45" s="7" t="inlineStr">
         <is>
-          <t>circularity_documents_impactOfSubstances[0]_category</t>
+          <t>circularity__documents__impactOfSubstances[0]__category</t>
         </is>
       </c>
       <c r="B45" s="7" t="inlineStr">
@@ -2584,7 +2584,7 @@
     <row r="46">
       <c r="A46" s="8" t="inlineStr">
         <is>
-          <t>circularity_documents_impactOfSubstances[0]_type</t>
+          <t>circularity__documents__impactOfSubstances[0]__type</t>
         </is>
       </c>
       <c r="B46" s="8" t="inlineStr">
@@ -2601,7 +2601,7 @@
     <row r="47">
       <c r="A47" s="7" t="inlineStr">
         <is>
-          <t>circularity_documents_impactOfSubstances[0]_header</t>
+          <t>circularity__documents__impactOfSubstances[0]__header</t>
         </is>
       </c>
       <c r="B47" s="7" t="inlineStr">
@@ -2614,7 +2614,7 @@
     <row r="48">
       <c r="A48" s="8" t="inlineStr">
         <is>
-          <t>circularity_documents_euTaxonomyDisclosureStatement[0]_content</t>
+          <t>circularity__documents__euTaxonomyDisclosureStatement[0]__content</t>
         </is>
       </c>
       <c r="B48" s="8" t="inlineStr">
@@ -2627,7 +2627,7 @@
     <row r="49">
       <c r="A49" s="7" t="inlineStr">
         <is>
-          <t>circularity_documents_euTaxonomyDisclosureStatement[0]_category</t>
+          <t>circularity__documents__euTaxonomyDisclosureStatement[0]__category</t>
         </is>
       </c>
       <c r="B49" s="7" t="inlineStr">
@@ -2655,7 +2655,7 @@
     <row r="50">
       <c r="A50" s="8" t="inlineStr">
         <is>
-          <t>circularity_documents_euTaxonomyDisclosureStatement[0]_type</t>
+          <t>circularity__documents__euTaxonomyDisclosureStatement[0]__type</t>
         </is>
       </c>
       <c r="B50" s="8" t="inlineStr">
@@ -2672,7 +2672,7 @@
     <row r="51">
       <c r="A51" s="7" t="inlineStr">
         <is>
-          <t>circularity_documents_euTaxonomyDisclosureStatement[0]_header</t>
+          <t>circularity__documents__euTaxonomyDisclosureStatement[0]__header</t>
         </is>
       </c>
       <c r="B51" s="7" t="inlineStr">
@@ -2685,7 +2685,7 @@
     <row r="52">
       <c r="A52" s="8" t="inlineStr">
         <is>
-          <t>circularity_documents_sustainabilityReport[0]_content</t>
+          <t>circularity__documents__sustainabilityReport[0]__content</t>
         </is>
       </c>
       <c r="B52" s="8" t="inlineStr">
@@ -2698,7 +2698,7 @@
     <row r="53">
       <c r="A53" s="7" t="inlineStr">
         <is>
-          <t>circularity_documents_sustainabilityReport[0]_category</t>
+          <t>circularity__documents__sustainabilityReport[0]__category</t>
         </is>
       </c>
       <c r="B53" s="7" t="inlineStr">
@@ -2726,7 +2726,7 @@
     <row r="54">
       <c r="A54" s="8" t="inlineStr">
         <is>
-          <t>circularity_documents_sustainabilityReport[0]_type</t>
+          <t>circularity__documents__sustainabilityReport[0]__type</t>
         </is>
       </c>
       <c r="B54" s="8" t="inlineStr">
@@ -2743,7 +2743,7 @@
     <row r="55">
       <c r="A55" s="7" t="inlineStr">
         <is>
-          <t>circularity_documents_sustainabilityReport[0]_header</t>
+          <t>circularity__documents__sustainabilityReport[0]__header</t>
         </is>
       </c>
       <c r="B55" s="7" t="inlineStr">
@@ -2756,7 +2756,7 @@
     <row r="56">
       <c r="A56" s="8" t="inlineStr">
         <is>
-          <t>circularity_documents_separateCollectionSymbol</t>
+          <t>circularity__documents__separateCollectionSymbol</t>
         </is>
       </c>
       <c r="B56" s="8" t="inlineStr">
@@ -2770,7 +2770,7 @@
     <row r="57">
       <c r="A57" s="7" t="inlineStr">
         <is>
-          <t>circularity_carbonFootprint[0]_value</t>
+          <t>circularity__carbonFootprint[0]__value</t>
         </is>
       </c>
       <c r="B57" s="7" t="inlineStr">
@@ -2786,7 +2786,7 @@
     <row r="58">
       <c r="A58" s="8" t="inlineStr">
         <is>
-          <t>circularity_carbonFootprint[0]_rulebook</t>
+          <t>circularity__carbonFootprint[0]__rulebook</t>
         </is>
       </c>
       <c r="B58" s="8" t="inlineStr">
@@ -2799,7 +2799,7 @@
     <row r="59">
       <c r="A59" s="7" t="inlineStr">
         <is>
-          <t>circularity_carbonFootprint[0]_lifecycle</t>
+          <t>circularity__carbonFootprint[0]__lifecycle</t>
         </is>
       </c>
       <c r="B59" s="7" t="inlineStr">
@@ -2812,7 +2812,7 @@
     <row r="60">
       <c r="A60" s="8" t="inlineStr">
         <is>
-          <t>circularity_carbonFootprint[0]_unit</t>
+          <t>circularity__carbonFootprint[0]__unit</t>
         </is>
       </c>
       <c r="B60" s="8" t="inlineStr">
@@ -2825,7 +2825,7 @@
     <row r="61">
       <c r="A61" s="7" t="inlineStr">
         <is>
-          <t>circularity_carbonFootprint[0]_type</t>
+          <t>circularity__carbonFootprint[0]__type</t>
         </is>
       </c>
       <c r="B61" s="7" t="inlineStr">
@@ -2844,7 +2844,7 @@
     <row r="62">
       <c r="A62" s="8" t="inlineStr">
         <is>
-          <t>circularity_carbonFootprint[0]_performanceClass</t>
+          <t>circularity__carbonFootprint[0]__performanceClass</t>
         </is>
       </c>
       <c r="B62" s="8" t="inlineStr">
@@ -2857,7 +2857,7 @@
     <row r="63">
       <c r="A63" s="7" t="inlineStr">
         <is>
-          <t>circularity_carbonFootprint[0]_manufacturingPlant</t>
+          <t>circularity__carbonFootprint[0]__manufacturingPlant</t>
         </is>
       </c>
       <c r="B63" s="7" t="inlineStr">
@@ -2870,7 +2870,7 @@
     <row r="64">
       <c r="A64" s="8" t="inlineStr">
         <is>
-          <t>circularity_carbonFootprint[0]_declaration</t>
+          <t>circularity__carbonFootprint[0]__declaration</t>
         </is>
       </c>
       <c r="B64" s="8" t="inlineStr">
@@ -2883,7 +2883,7 @@
     <row r="65">
       <c r="A65" s="7" t="inlineStr">
         <is>
-          <t>circularity_spareParts</t>
+          <t>circularity__spareParts</t>
         </is>
       </c>
       <c r="B65" s="7" t="inlineStr">
@@ -2896,7 +2896,7 @@
     <row r="66">
       <c r="A66" s="8" t="inlineStr">
         <is>
-          <t>circularity_status</t>
+          <t>circularity__status</t>
         </is>
       </c>
       <c r="B66" s="8" t="inlineStr">
@@ -2914,7 +2914,7 @@
     <row r="67">
       <c r="A67" s="7" t="inlineStr">
         <is>
-          <t>generalInformation_intoServiceDate</t>
+          <t>generalInformation__intoServiceDate</t>
         </is>
       </c>
       <c r="B67" s="7" t="inlineStr">
@@ -2930,7 +2930,7 @@
     <row r="68">
       <c r="A68" s="8" t="inlineStr">
         <is>
-          <t>generalInformation_manufacturer_facility</t>
+          <t>generalInformation__manufacturer__facility</t>
         </is>
       </c>
       <c r="B68" s="8" t="inlineStr">
@@ -2944,7 +2944,7 @@
     <row r="69">
       <c r="A69" s="7" t="inlineStr">
         <is>
-          <t>generalInformation_manufacturer_manufacturer</t>
+          <t>generalInformation__manufacturer__manufacturer</t>
         </is>
       </c>
       <c r="B69" s="7" t="inlineStr">
@@ -2958,7 +2958,7 @@
     <row r="70">
       <c r="A70" s="8" t="inlineStr">
         <is>
-          <t>generalInformation_manufacturer_manufacturingDate</t>
+          <t>generalInformation__manufacturer__manufacturingDate</t>
         </is>
       </c>
       <c r="B70" s="8" t="inlineStr">
@@ -2971,7 +2971,7 @@
     <row r="71">
       <c r="A71" s="7" t="inlineStr">
         <is>
-          <t>generalInformation_lifespan[0]_unit</t>
+          <t>generalInformation__lifespan[0]__unit</t>
         </is>
       </c>
       <c r="B71" s="7" t="inlineStr">
@@ -2988,7 +2988,7 @@
     <row r="72">
       <c r="A72" s="8" t="inlineStr">
         <is>
-          <t>generalInformation_lifespan[0]_value</t>
+          <t>generalInformation__lifespan[0]__value</t>
         </is>
       </c>
       <c r="B72" s="8" t="inlineStr">
@@ -3001,7 +3001,7 @@
     <row r="73">
       <c r="A73" s="7" t="inlineStr">
         <is>
-          <t>generalInformation_lifespan[0]_key</t>
+          <t>generalInformation__lifespan[0]__key</t>
         </is>
       </c>
       <c r="B73" s="7" t="inlineStr">
@@ -3019,7 +3019,7 @@
     <row r="74">
       <c r="A74" s="8" t="inlineStr">
         <is>
-          <t>sources[0]_content</t>
+          <t>sources[0]__content</t>
         </is>
       </c>
       <c r="B74" s="8" t="inlineStr">
@@ -3032,7 +3032,7 @@
     <row r="75">
       <c r="A75" s="7" t="inlineStr">
         <is>
-          <t>sources[0]_category</t>
+          <t>sources[0]__category</t>
         </is>
       </c>
       <c r="B75" s="7" t="inlineStr">
@@ -3060,7 +3060,7 @@
     <row r="76">
       <c r="A76" s="8" t="inlineStr">
         <is>
-          <t>sources[0]_type</t>
+          <t>sources[0]__type</t>
         </is>
       </c>
       <c r="B76" s="8" t="inlineStr">
@@ -3077,7 +3077,7 @@
     <row r="77">
       <c r="A77" s="7" t="inlineStr">
         <is>
-          <t>sources[0]_header</t>
+          <t>sources[0]__header</t>
         </is>
       </c>
       <c r="B77" s="7" t="inlineStr">
@@ -3090,7 +3090,7 @@
     <row r="78">
       <c r="A78" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_voltage_min</t>
+          <t>performance__rated__voltage__min</t>
         </is>
       </c>
       <c r="B78" s="8" t="inlineStr">
@@ -3104,7 +3104,7 @@
     <row r="79">
       <c r="A79" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_voltage_max</t>
+          <t>performance__rated__voltage__max</t>
         </is>
       </c>
       <c r="B79" s="7" t="inlineStr">
@@ -3118,7 +3118,7 @@
     <row r="80">
       <c r="A80" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_voltage_nominal</t>
+          <t>performance__rated__voltage__nominal</t>
         </is>
       </c>
       <c r="B80" s="8" t="inlineStr">
@@ -3132,7 +3132,7 @@
     <row r="81">
       <c r="A81" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_voltage_temperature</t>
+          <t>performance__rated__voltage__temperature</t>
         </is>
       </c>
       <c r="B81" s="7" t="inlineStr">
@@ -3145,7 +3145,7 @@
     <row r="82">
       <c r="A82" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_roundTripEfficiency_depthOfDischarge</t>
+          <t>performance__rated__roundTripEfficiency__depthOfDischarge</t>
         </is>
       </c>
       <c r="B82" s="8" t="inlineStr">
@@ -3159,7 +3159,7 @@
     <row r="83">
       <c r="A83" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_roundTripEfficiency_initial</t>
+          <t>performance__rated__roundTripEfficiency__initial</t>
         </is>
       </c>
       <c r="B83" s="7" t="inlineStr">
@@ -3173,7 +3173,7 @@
     <row r="84">
       <c r="A84" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_roundTripEfficiency_50PercentLife</t>
+          <t>performance__rated__roundTripEfficiency__50PercentLife</t>
         </is>
       </c>
       <c r="B84" s="8" t="inlineStr">
@@ -3187,7 +3187,7 @@
     <row r="85">
       <c r="A85" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_roundTripEfficiency_temperature</t>
+          <t>performance__rated__roundTripEfficiency__temperature</t>
         </is>
       </c>
       <c r="B85" s="7" t="inlineStr">
@@ -3200,7 +3200,7 @@
     <row r="86">
       <c r="A86" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_energy_value</t>
+          <t>performance__rated__energy__value</t>
         </is>
       </c>
       <c r="B86" s="8" t="inlineStr">
@@ -3213,7 +3213,7 @@
     <row r="87">
       <c r="A87" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_energy_temperature</t>
+          <t>performance__rated__energy__temperature</t>
         </is>
       </c>
       <c r="B87" s="7" t="inlineStr">
@@ -3226,7 +3226,7 @@
     <row r="88">
       <c r="A88" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_resistance_cell</t>
+          <t>performance__rated__resistance__cell</t>
         </is>
       </c>
       <c r="B88" s="8" t="inlineStr">
@@ -3242,7 +3242,7 @@
     <row r="89">
       <c r="A89" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_resistance_module</t>
+          <t>performance__rated__resistance__module</t>
         </is>
       </c>
       <c r="B89" s="7" t="inlineStr">
@@ -3255,7 +3255,7 @@
     <row r="90">
       <c r="A90" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_resistance_pack</t>
+          <t>performance__rated__resistance__pack</t>
         </is>
       </c>
       <c r="B90" s="8" t="inlineStr">
@@ -3271,7 +3271,7 @@
     <row r="91">
       <c r="A91" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_resistance_temperature</t>
+          <t>performance__rated__resistance__temperature</t>
         </is>
       </c>
       <c r="B91" s="7" t="inlineStr">
@@ -3284,7 +3284,7 @@
     <row r="92">
       <c r="A92" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_power_value</t>
+          <t>performance__rated__power__value</t>
         </is>
       </c>
       <c r="B92" s="8" t="inlineStr">
@@ -3297,7 +3297,7 @@
     <row r="93">
       <c r="A93" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_power_at20SoC</t>
+          <t>performance__rated__power__at20SoC</t>
         </is>
       </c>
       <c r="B93" s="7" t="inlineStr">
@@ -3311,7 +3311,7 @@
     <row r="94">
       <c r="A94" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_power_at80SoC</t>
+          <t>performance__rated__power__at80SoC</t>
         </is>
       </c>
       <c r="B94" s="8" t="inlineStr">
@@ -3325,7 +3325,7 @@
     <row r="95">
       <c r="A95" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_power_temperature</t>
+          <t>performance__rated__power__temperature</t>
         </is>
       </c>
       <c r="B95" s="7" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="96">
       <c r="A96" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_capacity_value</t>
+          <t>performance__rated__capacity__value</t>
         </is>
       </c>
       <c r="B96" s="8" t="inlineStr">
@@ -3351,7 +3351,7 @@
     <row r="97">
       <c r="A97" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_capacity_thresholdExhaustion</t>
+          <t>performance__rated__capacity__thresholdExhaustion</t>
         </is>
       </c>
       <c r="B97" s="7" t="inlineStr">
@@ -3365,7 +3365,7 @@
     <row r="98">
       <c r="A98" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_capacity_temperature</t>
+          <t>performance__rated__capacity__temperature</t>
         </is>
       </c>
       <c r="B98" s="8" t="inlineStr">
@@ -3378,7 +3378,7 @@
     <row r="99">
       <c r="A99" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_performanceDocument[0]_content</t>
+          <t>performance__rated__performanceDocument[0]__content</t>
         </is>
       </c>
       <c r="B99" s="7" t="inlineStr">
@@ -3391,7 +3391,7 @@
     <row r="100">
       <c r="A100" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_performanceDocument[0]_category</t>
+          <t>performance__rated__performanceDocument[0]__category</t>
         </is>
       </c>
       <c r="B100" s="8" t="inlineStr">
@@ -3419,7 +3419,7 @@
     <row r="101">
       <c r="A101" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_performanceDocument[0]_type</t>
+          <t>performance__rated__performanceDocument[0]__type</t>
         </is>
       </c>
       <c r="B101" s="7" t="inlineStr">
@@ -3436,7 +3436,7 @@
     <row r="102">
       <c r="A102" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_performanceDocument[0]_header</t>
+          <t>performance__rated__performanceDocument[0]__header</t>
         </is>
       </c>
       <c r="B102" s="8" t="inlineStr">
@@ -3449,7 +3449,7 @@
     <row r="103">
       <c r="A103" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_temperature_lower</t>
+          <t>performance__rated__temperature__lower</t>
         </is>
       </c>
       <c r="B103" s="7" t="inlineStr">
@@ -3463,7 +3463,7 @@
     <row r="104">
       <c r="A104" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_temperature_upper</t>
+          <t>performance__rated__temperature__upper</t>
         </is>
       </c>
       <c r="B104" s="8" t="inlineStr">
@@ -3477,7 +3477,7 @@
     <row r="105">
       <c r="A105" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_selfDischargingRate</t>
+          <t>performance__rated__selfDischargingRate</t>
         </is>
       </c>
       <c r="B105" s="7" t="inlineStr">
@@ -3491,7 +3491,7 @@
     <row r="106">
       <c r="A106" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_testReport[0]_content</t>
+          <t>performance__rated__testReport[0]__content</t>
         </is>
       </c>
       <c r="B106" s="8" t="inlineStr">
@@ -3504,7 +3504,7 @@
     <row r="107">
       <c r="A107" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_testReport[0]_category</t>
+          <t>performance__rated__testReport[0]__category</t>
         </is>
       </c>
       <c r="B107" s="7" t="inlineStr">
@@ -3532,7 +3532,7 @@
     <row r="108">
       <c r="A108" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_testReport[0]_type</t>
+          <t>performance__rated__testReport[0]__type</t>
         </is>
       </c>
       <c r="B108" s="8" t="inlineStr">
@@ -3549,7 +3549,7 @@
     <row r="109">
       <c r="A109" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_testReport[0]_header</t>
+          <t>performance__rated__testReport[0]__header</t>
         </is>
       </c>
       <c r="B109" s="7" t="inlineStr">
@@ -3562,7 +3562,7 @@
     <row r="110">
       <c r="A110" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_expectedYears</t>
+          <t>performance__rated__lifetime__expectedYears</t>
         </is>
       </c>
       <c r="B110" s="8" t="inlineStr">
@@ -3576,7 +3576,7 @@
     <row r="111">
       <c r="A111" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_report[0]_content</t>
+          <t>performance__rated__lifetime__report[0]__content</t>
         </is>
       </c>
       <c r="B111" s="7" t="inlineStr">
@@ -3589,7 +3589,7 @@
     <row r="112">
       <c r="A112" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_report[0]_category</t>
+          <t>performance__rated__lifetime__report[0]__category</t>
         </is>
       </c>
       <c r="B112" s="8" t="inlineStr">
@@ -3617,7 +3617,7 @@
     <row r="113">
       <c r="A113" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_report[0]_type</t>
+          <t>performance__rated__lifetime__report[0]__type</t>
         </is>
       </c>
       <c r="B113" s="7" t="inlineStr">
@@ -3634,7 +3634,7 @@
     <row r="114">
       <c r="A114" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_report[0]_header</t>
+          <t>performance__rated__lifetime__report[0]__header</t>
         </is>
       </c>
       <c r="B114" s="8" t="inlineStr">
@@ -3647,7 +3647,7 @@
     <row r="115">
       <c r="A115" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_cycleLifeTesting_temperature</t>
+          <t>performance__rated__lifetime__cycleLifeTesting__temperature</t>
         </is>
       </c>
       <c r="B115" s="7" t="inlineStr">
@@ -3660,7 +3660,7 @@
     <row r="116">
       <c r="A116" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_cycleLifeTesting_cycles</t>
+          <t>performance__rated__lifetime__cycleLifeTesting__cycles</t>
         </is>
       </c>
       <c r="B116" s="8" t="inlineStr">
@@ -3673,7 +3673,7 @@
     <row r="117">
       <c r="A117" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_cycleLifeTesting_depthOfDischarge</t>
+          <t>performance__rated__lifetime__cycleLifeTesting__depthOfDischarge</t>
         </is>
       </c>
       <c r="B117" s="7" t="inlineStr">
@@ -3687,7 +3687,7 @@
     <row r="118">
       <c r="A118" s="8" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_cycleLifeTesting_appliedChargeRate</t>
+          <t>performance__rated__lifetime__cycleLifeTesting__appliedChargeRate</t>
         </is>
       </c>
       <c r="B118" s="8" t="inlineStr">
@@ -3703,7 +3703,7 @@
     <row r="119">
       <c r="A119" s="7" t="inlineStr">
         <is>
-          <t>performance_rated_lifetime_cycleLifeTesting_appliedDischargeRate</t>
+          <t>performance__rated__lifetime__cycleLifeTesting__appliedDischargeRate</t>
         </is>
       </c>
       <c r="B119" s="7" t="inlineStr">
@@ -3719,7 +3719,7 @@
     <row r="120">
       <c r="A120" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_stateOfCharge_value</t>
+          <t>performance__dynamic__stateOfCharge__value</t>
         </is>
       </c>
       <c r="B120" s="8" t="inlineStr">
@@ -3732,7 +3732,7 @@
     <row r="121">
       <c r="A121" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_stateOfCharge_time</t>
+          <t>performance__dynamic__stateOfCharge__time</t>
         </is>
       </c>
       <c r="B121" s="7" t="inlineStr">
@@ -3746,7 +3746,7 @@
     <row r="122">
       <c r="A122" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_fullCycles_time</t>
+          <t>performance__dynamic__fullCycles__time</t>
         </is>
       </c>
       <c r="B122" s="8" t="inlineStr">
@@ -3760,7 +3760,7 @@
     <row r="123">
       <c r="A123" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_fullCycles_value</t>
+          <t>performance__dynamic__fullCycles__value</t>
         </is>
       </c>
       <c r="B123" s="7" t="inlineStr">
@@ -3773,7 +3773,7 @@
     <row r="124">
       <c r="A124" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_performanceDocument[0]_content</t>
+          <t>performance__dynamic__performanceDocument[0]__content</t>
         </is>
       </c>
       <c r="B124" s="8" t="inlineStr">
@@ -3786,7 +3786,7 @@
     <row r="125">
       <c r="A125" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_performanceDocument[0]_category</t>
+          <t>performance__dynamic__performanceDocument[0]__category</t>
         </is>
       </c>
       <c r="B125" s="7" t="inlineStr">
@@ -3814,7 +3814,7 @@
     <row r="126">
       <c r="A126" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_performanceDocument[0]_type</t>
+          <t>performance__dynamic__performanceDocument[0]__type</t>
         </is>
       </c>
       <c r="B126" s="8" t="inlineStr">
@@ -3831,7 +3831,7 @@
     <row r="127">
       <c r="A127" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_performanceDocument[0]_header</t>
+          <t>performance__dynamic__performanceDocument[0]__header</t>
         </is>
       </c>
       <c r="B127" s="7" t="inlineStr">
@@ -3844,7 +3844,7 @@
     <row r="128">
       <c r="A128" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_selfDischargingRate</t>
+          <t>performance__dynamic__selfDischargingRate</t>
         </is>
       </c>
       <c r="B128" s="8" t="inlineStr">
@@ -3858,7 +3858,7 @@
     <row r="129">
       <c r="A129" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_power_fade_value</t>
+          <t>performance__dynamic__power__fade__value</t>
         </is>
       </c>
       <c r="B129" s="7" t="inlineStr">
@@ -3871,7 +3871,7 @@
     <row r="130">
       <c r="A130" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_power_fade_time</t>
+          <t>performance__dynamic__power__fade__time</t>
         </is>
       </c>
       <c r="B130" s="8" t="inlineStr">
@@ -3885,7 +3885,7 @@
     <row r="131">
       <c r="A131" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_power_remaining_time</t>
+          <t>performance__dynamic__power__remaining__time</t>
         </is>
       </c>
       <c r="B131" s="7" t="inlineStr">
@@ -3899,7 +3899,7 @@
     <row r="132">
       <c r="A132" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_power_remaining_value</t>
+          <t>performance__dynamic__power__remaining__value</t>
         </is>
       </c>
       <c r="B132" s="8" t="inlineStr">
@@ -3912,7 +3912,7 @@
     <row r="133">
       <c r="A133" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_capacity_fade_value</t>
+          <t>performance__dynamic__capacity__fade__value</t>
         </is>
       </c>
       <c r="B133" s="7" t="inlineStr">
@@ -3925,7 +3925,7 @@
     <row r="134">
       <c r="A134" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_capacity_fade_time</t>
+          <t>performance__dynamic__capacity__fade__time</t>
         </is>
       </c>
       <c r="B134" s="8" t="inlineStr">
@@ -3939,7 +3939,7 @@
     <row r="135">
       <c r="A135" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_capacity_throughput_time</t>
+          <t>performance__dynamic__capacity__throughput__time</t>
         </is>
       </c>
       <c r="B135" s="7" t="inlineStr">
@@ -3953,7 +3953,7 @@
     <row r="136">
       <c r="A136" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_capacity_throughput_value</t>
+          <t>performance__dynamic__capacity__throughput__value</t>
         </is>
       </c>
       <c r="B136" s="8" t="inlineStr">
@@ -3966,7 +3966,7 @@
     <row r="137">
       <c r="A137" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_capacity_capacity_time</t>
+          <t>performance__dynamic__capacity__capacity__time</t>
         </is>
       </c>
       <c r="B137" s="7" t="inlineStr">
@@ -3980,7 +3980,7 @@
     <row r="138">
       <c r="A138" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_capacity_capacity_value</t>
+          <t>performance__dynamic__capacity__capacity__value</t>
         </is>
       </c>
       <c r="B138" s="8" t="inlineStr">
@@ -3993,7 +3993,7 @@
     <row r="139">
       <c r="A139" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_roundTripEfficiency_fade_value</t>
+          <t>performance__dynamic__roundTripEfficiency__fade__value</t>
         </is>
       </c>
       <c r="B139" s="7" t="inlineStr">
@@ -4006,7 +4006,7 @@
     <row r="140">
       <c r="A140" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_roundTripEfficiency_fade_time</t>
+          <t>performance__dynamic__roundTripEfficiency__fade__time</t>
         </is>
       </c>
       <c r="B140" s="8" t="inlineStr">
@@ -4020,7 +4020,7 @@
     <row r="141">
       <c r="A141" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_roundTripEfficiency_remaining_value</t>
+          <t>performance__dynamic__roundTripEfficiency__remaining__value</t>
         </is>
       </c>
       <c r="B141" s="7" t="inlineStr">
@@ -4033,7 +4033,7 @@
     <row r="142">
       <c r="A142" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_roundTripEfficiency_remaining_time</t>
+          <t>performance__dynamic__roundTripEfficiency__remaining__time</t>
         </is>
       </c>
       <c r="B142" s="8" t="inlineStr">
@@ -4047,7 +4047,7 @@
     <row r="143">
       <c r="A143" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_increase_pack_value</t>
+          <t>performance__dynamic__resistance__increase__pack__value</t>
         </is>
       </c>
       <c r="B143" s="7" t="inlineStr">
@@ -4060,7 +4060,7 @@
     <row r="144">
       <c r="A144" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_increase_pack_time</t>
+          <t>performance__dynamic__resistance__increase__pack__time</t>
         </is>
       </c>
       <c r="B144" s="8" t="inlineStr">
@@ -4074,7 +4074,7 @@
     <row r="145">
       <c r="A145" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_increase_module_value</t>
+          <t>performance__dynamic__resistance__increase__module__value</t>
         </is>
       </c>
       <c r="B145" s="7" t="inlineStr">
@@ -4087,7 +4087,7 @@
     <row r="146">
       <c r="A146" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_increase_module_time</t>
+          <t>performance__dynamic__resistance__increase__module__time</t>
         </is>
       </c>
       <c r="B146" s="8" t="inlineStr">
@@ -4101,7 +4101,7 @@
     <row r="147">
       <c r="A147" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_increase_cell_value</t>
+          <t>performance__dynamic__resistance__increase__cell__value</t>
         </is>
       </c>
       <c r="B147" s="7" t="inlineStr">
@@ -4114,7 +4114,7 @@
     <row r="148">
       <c r="A148" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_increase_cell_time</t>
+          <t>performance__dynamic__resistance__increase__cell__time</t>
         </is>
       </c>
       <c r="B148" s="8" t="inlineStr">
@@ -4128,7 +4128,7 @@
     <row r="149">
       <c r="A149" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_remaining_pack_time</t>
+          <t>performance__dynamic__resistance__remaining__pack__time</t>
         </is>
       </c>
       <c r="B149" s="7" t="inlineStr">
@@ -4142,7 +4142,7 @@
     <row r="150">
       <c r="A150" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_remaining_pack_value</t>
+          <t>performance__dynamic__resistance__remaining__pack__value</t>
         </is>
       </c>
       <c r="B150" s="8" t="inlineStr">
@@ -4155,7 +4155,7 @@
     <row r="151">
       <c r="A151" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_remaining_module_time</t>
+          <t>performance__dynamic__resistance__remaining__module__time</t>
         </is>
       </c>
       <c r="B151" s="7" t="inlineStr">
@@ -4169,7 +4169,7 @@
     <row r="152">
       <c r="A152" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_remaining_module_value</t>
+          <t>performance__dynamic__resistance__remaining__module__value</t>
         </is>
       </c>
       <c r="B152" s="8" t="inlineStr">
@@ -4182,7 +4182,7 @@
     <row r="153">
       <c r="A153" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_remaining_cell_time</t>
+          <t>performance__dynamic__resistance__remaining__cell__time</t>
         </is>
       </c>
       <c r="B153" s="7" t="inlineStr">
@@ -4196,7 +4196,7 @@
     <row r="154">
       <c r="A154" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_resistance_remaining_cell_value</t>
+          <t>performance__dynamic__resistance__remaining__cell__value</t>
         </is>
       </c>
       <c r="B154" s="8" t="inlineStr">
@@ -4209,7 +4209,7 @@
     <row r="155">
       <c r="A155" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_energy_soce_value</t>
+          <t>performance__dynamic__energy__soce__value</t>
         </is>
       </c>
       <c r="B155" s="7" t="inlineStr">
@@ -4222,7 +4222,7 @@
     <row r="156">
       <c r="A156" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_energy_soce_time</t>
+          <t>performance__dynamic__energy__soce__time</t>
         </is>
       </c>
       <c r="B156" s="8" t="inlineStr">
@@ -4236,7 +4236,7 @@
     <row r="157">
       <c r="A157" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_energy_remaining_time</t>
+          <t>performance__dynamic__energy__remaining__time</t>
         </is>
       </c>
       <c r="B157" s="7" t="inlineStr">
@@ -4250,7 +4250,7 @@
     <row r="158">
       <c r="A158" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_energy_remaining_value</t>
+          <t>performance__dynamic__energy__remaining__value</t>
         </is>
       </c>
       <c r="B158" s="8" t="inlineStr">
@@ -4263,7 +4263,7 @@
     <row r="159">
       <c r="A159" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_energy_throughput_time</t>
+          <t>performance__dynamic__energy__throughput__time</t>
         </is>
       </c>
       <c r="B159" s="7" t="inlineStr">
@@ -4277,7 +4277,7 @@
     <row r="160">
       <c r="A160" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_energy_throughput_value</t>
+          <t>performance__dynamic__energy__throughput__value</t>
         </is>
       </c>
       <c r="B160" s="8" t="inlineStr">
@@ -4290,7 +4290,7 @@
     <row r="161">
       <c r="A161" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_negativeEvents[0]_content</t>
+          <t>performance__dynamic__negativeEvents[0]__content</t>
         </is>
       </c>
       <c r="B161" s="7" t="inlineStr">
@@ -4303,7 +4303,7 @@
     <row r="162">
       <c r="A162" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_negativeEvents[0]_category</t>
+          <t>performance__dynamic__negativeEvents[0]__category</t>
         </is>
       </c>
       <c r="B162" s="8" t="inlineStr">
@@ -4331,7 +4331,7 @@
     <row r="163">
       <c r="A163" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_negativeEvents[0]_type</t>
+          <t>performance__dynamic__negativeEvents[0]__type</t>
         </is>
       </c>
       <c r="B163" s="7" t="inlineStr">
@@ -4348,7 +4348,7 @@
     <row r="164">
       <c r="A164" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_negativeEvents[0]_header</t>
+          <t>performance__dynamic__negativeEvents[0]__header</t>
         </is>
       </c>
       <c r="B164" s="8" t="inlineStr">
@@ -4361,7 +4361,7 @@
     <row r="165">
       <c r="A165" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_operatingEnvironment[0]_content</t>
+          <t>performance__dynamic__operatingEnvironment[0]__content</t>
         </is>
       </c>
       <c r="B165" s="7" t="inlineStr">
@@ -4374,7 +4374,7 @@
     <row r="166">
       <c r="A166" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_operatingEnvironment[0]_category</t>
+          <t>performance__dynamic__operatingEnvironment[0]__category</t>
         </is>
       </c>
       <c r="B166" s="8" t="inlineStr">
@@ -4402,7 +4402,7 @@
     <row r="167">
       <c r="A167" s="7" t="inlineStr">
         <is>
-          <t>performance_dynamic_operatingEnvironment[0]_type</t>
+          <t>performance__dynamic__operatingEnvironment[0]__type</t>
         </is>
       </c>
       <c r="B167" s="7" t="inlineStr">
@@ -4419,7 +4419,7 @@
     <row r="168">
       <c r="A168" s="8" t="inlineStr">
         <is>
-          <t>performance_dynamic_operatingEnvironment[0]_header</t>
+          <t>performance__dynamic__operatingEnvironment[0]__header</t>
         </is>
       </c>
       <c r="B168" s="8" t="inlineStr">
@@ -4432,7 +4432,7 @@
     <row r="169">
       <c r="A169" s="7" t="inlineStr">
         <is>
-          <t>conformity_declarationOfConformityId</t>
+          <t>conformity__declarationOfConformityId</t>
         </is>
       </c>
       <c r="B169" s="7" t="inlineStr">
@@ -4446,7 +4446,7 @@
     <row r="170">
       <c r="A170" s="8" t="inlineStr">
         <is>
-          <t>conformity_declarationOfConformity[0]_content</t>
+          <t>conformity__declarationOfConformity[0]__content</t>
         </is>
       </c>
       <c r="B170" s="8" t="inlineStr">
@@ -4459,7 +4459,7 @@
     <row r="171">
       <c r="A171" s="7" t="inlineStr">
         <is>
-          <t>conformity_declarationOfConformity[0]_category</t>
+          <t>conformity__declarationOfConformity[0]__category</t>
         </is>
       </c>
       <c r="B171" s="7" t="inlineStr">
@@ -4487,7 +4487,7 @@
     <row r="172">
       <c r="A172" s="8" t="inlineStr">
         <is>
-          <t>conformity_declarationOfConformity[0]_type</t>
+          <t>conformity__declarationOfConformity[0]__type</t>
         </is>
       </c>
       <c r="B172" s="8" t="inlineStr">
@@ -4504,7 +4504,7 @@
     <row r="173">
       <c r="A173" s="7" t="inlineStr">
         <is>
-          <t>conformity_declarationOfConformity[0]_header</t>
+          <t>conformity__declarationOfConformity[0]__header</t>
         </is>
       </c>
       <c r="B173" s="7" t="inlineStr">
@@ -4517,7 +4517,7 @@
     <row r="174">
       <c r="A174" s="8" t="inlineStr">
         <is>
-          <t>conformity_resultOfTestReport[0]_content</t>
+          <t>conformity__resultOfTestReport[0]__content</t>
         </is>
       </c>
       <c r="B174" s="8" t="inlineStr">
@@ -4530,7 +4530,7 @@
     <row r="175">
       <c r="A175" s="7" t="inlineStr">
         <is>
-          <t>conformity_resultOfTestReport[0]_category</t>
+          <t>conformity__resultOfTestReport[0]__category</t>
         </is>
       </c>
       <c r="B175" s="7" t="inlineStr">
@@ -4558,7 +4558,7 @@
     <row r="176">
       <c r="A176" s="8" t="inlineStr">
         <is>
-          <t>conformity_resultOfTestReport[0]_type</t>
+          <t>conformity__resultOfTestReport[0]__type</t>
         </is>
       </c>
       <c r="B176" s="8" t="inlineStr">
@@ -4575,7 +4575,7 @@
     <row r="177">
       <c r="A177" s="7" t="inlineStr">
         <is>
-          <t>conformity_resultOfTestReport[0]_header</t>
+          <t>conformity__resultOfTestReport[0]__header</t>
         </is>
       </c>
       <c r="B177" s="7" t="inlineStr">
@@ -4588,7 +4588,7 @@
     <row r="178">
       <c r="A178" s="8" t="inlineStr">
         <is>
-          <t>conformity_thirdPartyAssurance[0]_content</t>
+          <t>conformity__thirdPartyAssurance[0]__content</t>
         </is>
       </c>
       <c r="B178" s="8" t="inlineStr">
@@ -4601,7 +4601,7 @@
     <row r="179">
       <c r="A179" s="7" t="inlineStr">
         <is>
-          <t>conformity_thirdPartyAssurance[0]_category</t>
+          <t>conformity__thirdPartyAssurance[0]__category</t>
         </is>
       </c>
       <c r="B179" s="7" t="inlineStr">
@@ -4629,7 +4629,7 @@
     <row r="180">
       <c r="A180" s="8" t="inlineStr">
         <is>
-          <t>conformity_thirdPartyAssurance[0]_type</t>
+          <t>conformity__thirdPartyAssurance[0]__type</t>
         </is>
       </c>
       <c r="B180" s="8" t="inlineStr">
@@ -4646,7 +4646,7 @@
     <row r="181">
       <c r="A181" s="7" t="inlineStr">
         <is>
-          <t>conformity_thirdPartyAssurance[0]_header</t>
+          <t>conformity__thirdPartyAssurance[0]__header</t>
         </is>
       </c>
       <c r="B181" s="7" t="inlineStr">
@@ -4659,7 +4659,7 @@
     <row r="182">
       <c r="A182" s="8" t="inlineStr">
         <is>
-          <t>conformity_dueDiligencePolicy[0]_content</t>
+          <t>conformity__dueDiligencePolicy[0]__content</t>
         </is>
       </c>
       <c r="B182" s="8" t="inlineStr">
@@ -4672,7 +4672,7 @@
     <row r="183">
       <c r="A183" s="7" t="inlineStr">
         <is>
-          <t>conformity_dueDiligencePolicy[0]_category</t>
+          <t>conformity__dueDiligencePolicy[0]__category</t>
         </is>
       </c>
       <c r="B183" s="7" t="inlineStr">
@@ -4700,7 +4700,7 @@
     <row r="184">
       <c r="A184" s="8" t="inlineStr">
         <is>
-          <t>conformity_dueDiligencePolicy[0]_type</t>
+          <t>conformity__dueDiligencePolicy[0]__type</t>
         </is>
       </c>
       <c r="B184" s="8" t="inlineStr">
@@ -4717,7 +4717,7 @@
     <row r="185">
       <c r="A185" s="7" t="inlineStr">
         <is>
-          <t>conformity_dueDiligencePolicy[0]_header</t>
+          <t>conformity__dueDiligencePolicy[0]__header</t>
         </is>
       </c>
       <c r="B185" s="7" t="inlineStr">
@@ -4730,7 +4730,7 @@
     <row r="186">
       <c r="A186" s="8" t="inlineStr">
         <is>
-          <t>safety_usableExtinguishAgent[0]_document[0]_content</t>
+          <t>safety__usableExtinguishAgent[0]__document[0]__content</t>
         </is>
       </c>
       <c r="B186" s="8" t="inlineStr">
@@ -4743,7 +4743,7 @@
     <row r="187">
       <c r="A187" s="7" t="inlineStr">
         <is>
-          <t>safety_usableExtinguishAgent[0]_document[0]_category</t>
+          <t>safety__usableExtinguishAgent[0]__document[0]__category</t>
         </is>
       </c>
       <c r="B187" s="7" t="inlineStr">
@@ -4771,7 +4771,7 @@
     <row r="188">
       <c r="A188" s="8" t="inlineStr">
         <is>
-          <t>safety_usableExtinguishAgent[0]_document[0]_type</t>
+          <t>safety__usableExtinguishAgent[0]__document[0]__type</t>
         </is>
       </c>
       <c r="B188" s="8" t="inlineStr">
@@ -4788,7 +4788,7 @@
     <row r="189">
       <c r="A189" s="7" t="inlineStr">
         <is>
-          <t>safety_usableExtinguishAgent[0]_document[0]_header</t>
+          <t>safety__usableExtinguishAgent[0]__document[0]__header</t>
         </is>
       </c>
       <c r="B189" s="7" t="inlineStr">
@@ -4801,7 +4801,7 @@
     <row r="190">
       <c r="A190" s="8" t="inlineStr">
         <is>
-          <t>safety_usableExtinguishAgent[0]_media</t>
+          <t>safety__usableExtinguishAgent[0]__media</t>
         </is>
       </c>
       <c r="B190" s="8" t="inlineStr">
@@ -4815,7 +4815,7 @@
     <row r="191">
       <c r="A191" s="7" t="inlineStr">
         <is>
-          <t>safety_usableExtinguishAgent[0]_fireClass</t>
+          <t>safety__usableExtinguishAgent[0]__fireClass</t>
         </is>
       </c>
       <c r="B191" s="7" t="inlineStr">
@@ -4828,7 +4828,7 @@
     <row r="192">
       <c r="A192" s="8" t="inlineStr">
         <is>
-          <t>safety_safetyMeasures[0]_content</t>
+          <t>safety__safetyMeasures[0]__content</t>
         </is>
       </c>
       <c r="B192" s="8" t="inlineStr">
@@ -4841,7 +4841,7 @@
     <row r="193">
       <c r="A193" s="7" t="inlineStr">
         <is>
-          <t>safety_safetyMeasures[0]_category</t>
+          <t>safety__safetyMeasures[0]__category</t>
         </is>
       </c>
       <c r="B193" s="7" t="inlineStr">
@@ -4869,7 +4869,7 @@
     <row r="194">
       <c r="A194" s="8" t="inlineStr">
         <is>
-          <t>safety_safetyMeasures[0]_type</t>
+          <t>safety__safetyMeasures[0]__type</t>
         </is>
       </c>
       <c r="B194" s="8" t="inlineStr">
@@ -4886,7 +4886,7 @@
     <row r="195">
       <c r="A195" s="7" t="inlineStr">
         <is>
-          <t>safety_safetyMeasures[0]_header</t>
+          <t>safety__safetyMeasures[0]__header</t>
         </is>
       </c>
       <c r="B195" s="7" t="inlineStr">
@@ -4899,7 +4899,7 @@
     <row r="196">
       <c r="A196" s="8" t="inlineStr">
         <is>
-          <t>safety_meaningOfLabels[0]_content</t>
+          <t>safety__meaningOfLabels[0]__content</t>
         </is>
       </c>
       <c r="B196" s="8" t="inlineStr">
@@ -4912,7 +4912,7 @@
     <row r="197">
       <c r="A197" s="7" t="inlineStr">
         <is>
-          <t>safety_meaningOfLabels[0]_category</t>
+          <t>safety__meaningOfLabels[0]__category</t>
         </is>
       </c>
       <c r="B197" s="7" t="inlineStr">
@@ -4940,7 +4940,7 @@
     <row r="198">
       <c r="A198" s="8" t="inlineStr">
         <is>
-          <t>safety_meaningOfLabels[0]_type</t>
+          <t>safety__meaningOfLabels[0]__type</t>
         </is>
       </c>
       <c r="B198" s="8" t="inlineStr">
@@ -4957,7 +4957,7 @@
     <row r="199">
       <c r="A199" s="7" t="inlineStr">
         <is>
-          <t>safety_meaningOfLabels[0]_header</t>
+          <t>safety__meaningOfLabels[0]__header</t>
         </is>
       </c>
       <c r="B199" s="7" t="inlineStr">
@@ -4970,7 +4970,7 @@
     <row r="200">
       <c r="A200" s="8" t="inlineStr">
         <is>
-          <t>safety_safeDischarging[0]_content</t>
+          <t>safety__safeDischarging[0]__content</t>
         </is>
       </c>
       <c r="B200" s="8" t="inlineStr">
@@ -4983,7 +4983,7 @@
     <row r="201">
       <c r="A201" s="7" t="inlineStr">
         <is>
-          <t>safety_safeDischarging[0]_category</t>
+          <t>safety__safeDischarging[0]__category</t>
         </is>
       </c>
       <c r="B201" s="7" t="inlineStr">
@@ -5011,7 +5011,7 @@
     <row r="202">
       <c r="A202" s="8" t="inlineStr">
         <is>
-          <t>safety_safeDischarging[0]_type</t>
+          <t>safety__safeDischarging[0]__type</t>
         </is>
       </c>
       <c r="B202" s="8" t="inlineStr">
@@ -5028,7 +5028,7 @@
     <row r="203">
       <c r="A203" s="7" t="inlineStr">
         <is>
-          <t>safety_safeDischarging[0]_header</t>
+          <t>safety__safeDischarging[0]__header</t>
         </is>
       </c>
       <c r="B203" s="7" t="inlineStr">
@@ -5041,7 +5041,7 @@
     <row r="204">
       <c r="A204" s="8" t="inlineStr">
         <is>
-          <t>safety_dismantling[0]_content</t>
+          <t>safety__dismantling[0]__content</t>
         </is>
       </c>
       <c r="B204" s="8" t="inlineStr">
@@ -5054,7 +5054,7 @@
     <row r="205">
       <c r="A205" s="7" t="inlineStr">
         <is>
-          <t>safety_dismantling[0]_category</t>
+          <t>safety__dismantling[0]__category</t>
         </is>
       </c>
       <c r="B205" s="7" t="inlineStr">
@@ -5082,7 +5082,7 @@
     <row r="206">
       <c r="A206" s="8" t="inlineStr">
         <is>
-          <t>safety_dismantling[0]_type</t>
+          <t>safety__dismantling[0]__type</t>
         </is>
       </c>
       <c r="B206" s="8" t="inlineStr">
@@ -5099,7 +5099,7 @@
     <row r="207">
       <c r="A207" s="7" t="inlineStr">
         <is>
-          <t>safety_dismantling[0]_header</t>
+          <t>safety__dismantling[0]__header</t>
         </is>
       </c>
       <c r="B207" s="7" t="inlineStr">
@@ -5112,7 +5112,7 @@
     <row r="208">
       <c r="A208" s="8" t="inlineStr">
         <is>
-          <t>safety_removalFromAppliance[0]_content</t>
+          <t>safety__removalFromAppliance[0]__content</t>
         </is>
       </c>
       <c r="B208" s="8" t="inlineStr">
@@ -5125,7 +5125,7 @@
     <row r="209">
       <c r="A209" s="7" t="inlineStr">
         <is>
-          <t>safety_removalFromAppliance[0]_category</t>
+          <t>safety__removalFromAppliance[0]__category</t>
         </is>
       </c>
       <c r="B209" s="7" t="inlineStr">
@@ -5153,7 +5153,7 @@
     <row r="210">
       <c r="A210" s="8" t="inlineStr">
         <is>
-          <t>safety_removalFromAppliance[0]_type</t>
+          <t>safety__removalFromAppliance[0]__type</t>
         </is>
       </c>
       <c r="B210" s="8" t="inlineStr">
@@ -5170,7 +5170,7 @@
     <row r="211">
       <c r="A211" s="7" t="inlineStr">
         <is>
-          <t>safety_removalFromAppliance[0]_header</t>
+          <t>safety__removalFromAppliance[0]__header</t>
         </is>
       </c>
       <c r="B211" s="7" t="inlineStr">
@@ -5183,7 +5183,7 @@
     <row r="212">
       <c r="A212" s="8" t="inlineStr">
         <is>
-          <t>physicalDimension_weight_value</t>
+          <t>physicalDimension__weight__value</t>
         </is>
       </c>
       <c r="B212" s="8" t="inlineStr">
@@ -5196,7 +5196,7 @@
     <row r="213">
       <c r="A213" s="7" t="inlineStr">
         <is>
-          <t>physicalDimension_weight_unit</t>
+          <t>physicalDimension__weight__unit</t>
         </is>
       </c>
       <c r="B213" s="7" t="inlineStr">
@@ -5213,7 +5213,7 @@
     <row r="214">
       <c r="A214" s="8" t="inlineStr">
         <is>
-          <t>physicalDimension_volume_value</t>
+          <t>physicalDimension__volume__value</t>
         </is>
       </c>
       <c r="B214" s="8" t="inlineStr">
@@ -5226,7 +5226,7 @@
     <row r="215">
       <c r="A215" s="7" t="inlineStr">
         <is>
-          <t>physicalDimension_volume_unit</t>
+          <t>physicalDimension__volume__unit</t>
         </is>
       </c>
       <c r="B215" s="7" t="inlineStr">
@@ -5243,7 +5243,7 @@
     <row r="216">
       <c r="A216" s="8" t="inlineStr">
         <is>
-          <t>physicalDimension_height_value</t>
+          <t>physicalDimension__height__value</t>
         </is>
       </c>
       <c r="B216" s="8" t="inlineStr">
@@ -5256,7 +5256,7 @@
     <row r="217">
       <c r="A217" s="7" t="inlineStr">
         <is>
-          <t>physicalDimension_height_unit</t>
+          <t>physicalDimension__height__unit</t>
         </is>
       </c>
       <c r="B217" s="7" t="inlineStr">
@@ -5273,7 +5273,7 @@
     <row r="218">
       <c r="A218" s="8" t="inlineStr">
         <is>
-          <t>physicalDimension_diameter_value</t>
+          <t>physicalDimension__diameter__value</t>
         </is>
       </c>
       <c r="B218" s="8" t="inlineStr">
@@ -5286,7 +5286,7 @@
     <row r="219">
       <c r="A219" s="7" t="inlineStr">
         <is>
-          <t>physicalDimension_diameter_unit</t>
+          <t>physicalDimension__diameter__unit</t>
         </is>
       </c>
       <c r="B219" s="7" t="inlineStr">
@@ -5303,7 +5303,7 @@
     <row r="220">
       <c r="A220" s="8" t="inlineStr">
         <is>
-          <t>physicalDimension_length_value</t>
+          <t>physicalDimension__length__value</t>
         </is>
       </c>
       <c r="B220" s="8" t="inlineStr">
@@ -5316,7 +5316,7 @@
     <row r="221">
       <c r="A221" s="7" t="inlineStr">
         <is>
-          <t>physicalDimension_length_unit</t>
+          <t>physicalDimension__length__unit</t>
         </is>
       </c>
       <c r="B221" s="7" t="inlineStr">
@@ -5333,7 +5333,7 @@
     <row r="222">
       <c r="A222" s="8" t="inlineStr">
         <is>
-          <t>physicalDimension_width_value</t>
+          <t>physicalDimension__width__value</t>
         </is>
       </c>
       <c r="B222" s="8" t="inlineStr">
@@ -5346,7 +5346,7 @@
     <row r="223">
       <c r="A223" s="7" t="inlineStr">
         <is>
-          <t>physicalDimension_width_unit</t>
+          <t>physicalDimension__width__unit</t>
         </is>
       </c>
       <c r="B223" s="7" t="inlineStr">
@@ -5363,7 +5363,7 @@
     <row r="224">
       <c r="A224" s="8" t="inlineStr">
         <is>
-          <t>metadata_version</t>
+          <t>metadata__version</t>
         </is>
       </c>
       <c r="B224" s="8" t="inlineStr">
@@ -5376,7 +5376,7 @@
     <row r="225">
       <c r="A225" s="7" t="inlineStr">
         <is>
-          <t>metadata_status</t>
+          <t>metadata__status</t>
         </is>
       </c>
       <c r="B225" s="7" t="inlineStr">
@@ -5393,7 +5393,7 @@
     <row r="226">
       <c r="A226" s="8" t="inlineStr">
         <is>
-          <t>metadata_expirationDate</t>
+          <t>metadata__expirationDate</t>
         </is>
       </c>
       <c r="B226" s="8" t="inlineStr">
@@ -5407,7 +5407,7 @@
     <row r="227">
       <c r="A227" s="7" t="inlineStr">
         <is>
-          <t>metadata_issueDate</t>
+          <t>metadata__issueDate</t>
         </is>
       </c>
       <c r="B227" s="7" t="inlineStr">
@@ -5420,7 +5420,7 @@
     <row r="228">
       <c r="A228" s="8" t="inlineStr">
         <is>
-          <t>metadata_economicOperator_economicOperatorId</t>
+          <t>metadata__economicOperator__economicOperatorId</t>
         </is>
       </c>
       <c r="B228" s="8" t="inlineStr">
@@ -5434,7 +5434,7 @@
     <row r="229">
       <c r="A229" s="7" t="inlineStr">
         <is>
-          <t>metadata_predecessor</t>
+          <t>metadata__predecessor</t>
         </is>
       </c>
       <c r="B229" s="7" t="inlineStr">
@@ -5447,7 +5447,7 @@
     <row r="230">
       <c r="A230" s="8" t="inlineStr">
         <is>
-          <t>metadata_passportIdentifier</t>
+          <t>metadata__passportIdentifier</t>
         </is>
       </c>
       <c r="B230" s="8" t="inlineStr">

</xml_diff>

<commit_message>
update display name for dtwin id so as to avoid duplicating column names in reporting templates with aspect model col names
</commit_message>
<xml_diff>
--- a/excel_reporting_templates/BatteryPass-4.0.0-schema-reporting_template.xlsx
+++ b/excel_reporting_templates/BatteryPass-4.0.0-schema-reporting_template.xlsx
@@ -484,7 +484,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="2.4" customWidth="1" min="1" max="1"/>
+    <col width="9.6" customWidth="1" min="1" max="1"/>
     <col width="21.6" customWidth="1" min="2" max="2"/>
     <col width="16.8" customWidth="1" min="3" max="3"/>
     <col width="28.8" customWidth="1" min="4" max="4"/>
@@ -715,7 +715,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>dtwin_id</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -1915,7 +1915,7 @@
     <row r="5">
       <c r="A5" s="7" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>dtwin_id</t>
         </is>
       </c>
       <c r="B5" s="7" t="inlineStr">
@@ -5501,7 +5501,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ecb7538e63b08669e9b1ce35481507168308c414</t>
+          <t>41f43fae0e26ae5cfe94c2ce213309dcee6a0803</t>
         </is>
       </c>
     </row>
@@ -5513,7 +5513,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://github.com/dataspacesolutions/sldt-semantic-models/commit/ecb7538e63b08669e9b1ce35481507168308c414</t>
+          <t>https://github.com/dataspacesolutions/sldt-semantic-models/commit/41f43fae0e26ae5cfe94c2ce213309dcee6a0803</t>
         </is>
       </c>
     </row>
@@ -5525,7 +5525,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-02-01 10:20:11+00:00</t>
+          <t>2025-03-10 14:48:29+00:00</t>
         </is>
       </c>
     </row>
@@ -5537,7 +5537,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Adding generated artifacts for new models</t>
+          <t>Adding auto-generated artifacts for new models</t>
         </is>
       </c>
     </row>

</xml_diff>